<commit_message>
CIERRE 24 SEPT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/BALANCE ABASTOS   AGOSTO       2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/BALANCE ABASTOS   AGOSTO       2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="14" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="16" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O     2 0 2 1    " sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="840">
   <si>
     <t>MORRALLA EN CAJA DE 11 SUR   2,800.00  +  $ 1,200.00 Total    $  4,000.00</t>
   </si>
@@ -3047,6 +3047,48 @@
   </si>
   <si>
     <t>total de FALTANTE</t>
+  </si>
+  <si>
+    <t>AGOSTO.,</t>
+  </si>
+  <si>
+    <t>SERV CAMARA</t>
+  </si>
+  <si>
+    <t>Reinst Basculas</t>
+  </si>
+  <si>
+    <t>ROLLOS BASCULAS</t>
+  </si>
+  <si>
+    <t>ETIQUETADORA</t>
+  </si>
+  <si>
+    <t>PRESTAMO 3/18</t>
+  </si>
+  <si>
+    <t>INTERESES S/Prest 3/18</t>
+  </si>
+  <si>
+    <t>TARJETA +  SSD</t>
+  </si>
+  <si>
+    <t>IMPUESTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESECHABLES </t>
+  </si>
+  <si>
+    <t>COMISION AFILIACION</t>
+  </si>
+  <si>
+    <t>3%  IMPUESTO</t>
+  </si>
+  <si>
+    <t>GARANTIA FIRA  4</t>
+  </si>
+  <si>
+    <t>INERNET</t>
   </si>
 </sst>
 </file>
@@ -4933,7 +4975,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="656">
+  <cellXfs count="659">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6039,31 +6081,45 @@
     <xf numFmtId="0" fontId="17" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="7" fillId="16" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="16" borderId="80" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="16" borderId="81" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="16" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="16" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="16" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="16" borderId="83" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="94" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6105,26 +6161,31 @@
     <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="15" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6139,14 +6200,14 @@
     <xf numFmtId="166" fontId="6" fillId="15" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="35" fillId="10" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6165,6 +6226,15 @@
     </xf>
     <xf numFmtId="44" fontId="35" fillId="10" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -6244,26 +6314,32 @@
     <xf numFmtId="44" fontId="49" fillId="0" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="44" fontId="53" fillId="20" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="8" borderId="67" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6304,32 +6380,53 @@
     <xf numFmtId="44" fontId="16" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="16" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="6" fillId="11" borderId="73" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="6" fillId="11" borderId="85" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="6" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="6" fillId="11" borderId="87" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="35" fillId="7" borderId="96" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="35" fillId="7" borderId="97" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="35" fillId="7" borderId="99" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="35" fillId="7" borderId="100" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="8" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="8" borderId="95" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="7" borderId="98" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="7" fillId="7" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="53" fillId="20" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="8" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -6343,6 +6440,18 @@
     <xf numFmtId="44" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="35" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="35" fillId="11" borderId="87" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="35" fillId="11" borderId="88" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="35" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6351,6 +6460,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="87" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="88" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="7" fontId="35" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6373,84 +6494,14 @@
     <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="87" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="88" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="16" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="7" fillId="16" borderId="80" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="7" fillId="16" borderId="81" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="7" fillId="16" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="7" fillId="16" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="16" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="7" fillId="16" borderId="83" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="35" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="35" fillId="11" borderId="87" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="35" fillId="11" borderId="88" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="35" fillId="11" borderId="89" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="6" fillId="11" borderId="73" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="7" fontId="6" fillId="11" borderId="85" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="94" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="7" fontId="6" fillId="11" borderId="86" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="6" fillId="11" borderId="87" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="8" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="8" borderId="95" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="35" fillId="7" borderId="96" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="35" fillId="7" borderId="97" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="7" borderId="98" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="35" fillId="7" borderId="99" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="35" fillId="7" borderId="100" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="7" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -12105,17 +12156,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="535" t="s">
+      <c r="C1" s="524" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="535"/>
-      <c r="E1" s="535"/>
-      <c r="F1" s="535"/>
-      <c r="G1" s="535"/>
-      <c r="H1" s="535"/>
-      <c r="I1" s="535"/>
-      <c r="J1" s="535"/>
-      <c r="K1" s="535"/>
+      <c r="D1" s="524"/>
+      <c r="E1" s="524"/>
+      <c r="F1" s="524"/>
+      <c r="G1" s="524"/>
+      <c r="H1" s="524"/>
+      <c r="I1" s="524"/>
+      <c r="J1" s="524"/>
+      <c r="K1" s="524"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -12146,17 +12197,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="536" t="s">
+      <c r="B3" s="525" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="537"/>
+      <c r="C3" s="526"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="538" t="s">
+      <c r="H3" s="527" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="538"/>
+      <c r="I3" s="527"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -12185,14 +12236,14 @@
       <c r="D4" s="23">
         <v>44201</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="528" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="529"/>
+      <c r="H4" s="530" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="531"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -14803,61 +14854,61 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="522" t="s">
+      <c r="H64" s="532" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="523"/>
+      <c r="I64" s="533"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="524">
+      <c r="K64" s="534">
         <f>I62+L62</f>
         <v>360753.85</v>
       </c>
-      <c r="L64" s="525"/>
-      <c r="M64" s="526">
+      <c r="L64" s="535"/>
+      <c r="M64" s="536">
         <f>M62+N62</f>
         <v>2886514.7</v>
       </c>
-      <c r="N64" s="527"/>
+      <c r="N64" s="537"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="534" t="s">
+      <c r="D65" s="544" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="534"/>
+      <c r="E65" s="544"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2365880.5699999998</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="513">
+      <c r="P65" s="545">
         <f>P62+Q62</f>
         <v>3321521.28</v>
       </c>
-      <c r="Q65" s="514"/>
+      <c r="Q65" s="546"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="515" t="s">
+      <c r="D66" s="547" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="515"/>
+      <c r="E66" s="547"/>
       <c r="F66" s="95">
         <v>-2276696.6800000002</v>
       </c>
-      <c r="I66" s="516" t="s">
+      <c r="I66" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="517"/>
-      <c r="K66" s="518">
+      <c r="J66" s="549"/>
+      <c r="K66" s="550">
         <f>F68+F69+F70</f>
         <v>344253.98999999964</v>
       </c>
-      <c r="L66" s="519"/>
+      <c r="L66" s="551"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
@@ -14891,11 +14942,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="520">
+      <c r="K68" s="552">
         <f>-C4</f>
         <v>-250864.68</v>
       </c>
-      <c r="L68" s="521"/>
+      <c r="L68" s="553"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -14919,22 +14970,22 @@
       <c r="C70" s="119">
         <v>44230</v>
       </c>
-      <c r="D70" s="528" t="s">
+      <c r="D70" s="538" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="529"/>
+      <c r="E70" s="539"/>
       <c r="F70" s="120">
         <v>209541.1</v>
       </c>
-      <c r="I70" s="530" t="s">
+      <c r="I70" s="540" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="531"/>
-      <c r="K70" s="532">
+      <c r="J70" s="541"/>
+      <c r="K70" s="542">
         <f>K66+K68</f>
         <v>93389.309999999648</v>
       </c>
-      <c r="L70" s="533"/>
+      <c r="L70" s="543"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -15038,11 +15089,11 @@
     <sortCondition ref="J35:J54"/>
   </sortState>
   <mergeCells count="17">
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P65:Q65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K68:L68"/>
     <mergeCell ref="H64:I64"/>
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="M64:N64"/>
@@ -15050,11 +15101,11 @@
     <mergeCell ref="I70:J70"/>
     <mergeCell ref="K70:L70"/>
     <mergeCell ref="D65:E65"/>
-    <mergeCell ref="P65:Q65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.2" right="0.16" top="0.34" bottom="0.32" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -16479,20 +16530,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="567" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="535" t="s">
+      <c r="C1" s="524" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="535"/>
-      <c r="E1" s="535"/>
-      <c r="F1" s="535"/>
-      <c r="G1" s="535"/>
-      <c r="H1" s="535"/>
-      <c r="I1" s="535"/>
-      <c r="J1" s="535"/>
-      <c r="K1" s="535"/>
+      <c r="D1" s="524"/>
+      <c r="E1" s="524"/>
+      <c r="F1" s="524"/>
+      <c r="G1" s="524"/>
+      <c r="H1" s="524"/>
+      <c r="I1" s="524"/>
+      <c r="J1" s="524"/>
+      <c r="K1" s="524"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -16502,7 +16553,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="568"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -16521,27 +16572,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="566" t="s">
+      <c r="AB2" s="580" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="566"/>
-      <c r="AD2" s="566"/>
-      <c r="AE2" s="566"/>
-      <c r="AF2" s="566"/>
-      <c r="AG2" s="566"/>
+      <c r="AC2" s="580"/>
+      <c r="AD2" s="580"/>
+      <c r="AE2" s="580"/>
+      <c r="AF2" s="580"/>
+      <c r="AG2" s="580"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="536" t="s">
+      <c r="B3" s="525" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="537"/>
+      <c r="C3" s="526"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="538" t="s">
+      <c r="H3" s="527" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="538"/>
+      <c r="I3" s="527"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -16549,7 +16600,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="556" t="s">
+      <c r="P3" s="570" t="s">
         <v>562</v>
       </c>
       <c r="Q3" s="393"/>
@@ -16562,12 +16613,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="566"/>
-      <c r="AC3" s="566"/>
-      <c r="AD3" s="566"/>
-      <c r="AE3" s="566"/>
-      <c r="AF3" s="566"/>
-      <c r="AG3" s="566"/>
+      <c r="AB3" s="580"/>
+      <c r="AC3" s="580"/>
+      <c r="AD3" s="580"/>
+      <c r="AE3" s="580"/>
+      <c r="AF3" s="580"/>
+      <c r="AG3" s="580"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -16580,14 +16631,14 @@
       <c r="D4" s="23">
         <v>44353</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="528" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="529"/>
+      <c r="H4" s="530" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="531"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -16598,7 +16649,7 @@
         <v>10</v>
       </c>
       <c r="O4" s="365"/>
-      <c r="P4" s="556"/>
+      <c r="P4" s="570"/>
       <c r="Q4" s="393"/>
       <c r="R4" s="30"/>
       <c r="S4" s="31"/>
@@ -16613,16 +16664,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="567" t="s">
+      <c r="AB4" s="581" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="568"/>
+      <c r="AC4" s="582"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="569" t="s">
+      <c r="AE4" s="583" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="569"/>
-      <c r="AG4" s="569"/>
+      <c r="AF4" s="583"/>
+      <c r="AG4" s="583"/>
     </row>
     <row r="5" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
@@ -18034,10 +18085,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="574" t="s">
+      <c r="AE23" s="588" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="575"/>
+      <c r="AF23" s="589"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -18181,11 +18232,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="576" t="s">
+      <c r="AE25" s="590" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="577"/>
-      <c r="AG25" s="580">
+      <c r="AF25" s="591"/>
+      <c r="AG25" s="594">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -18256,9 +18307,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="578"/>
-      <c r="AF26" s="579"/>
-      <c r="AG26" s="581"/>
+      <c r="AE26" s="592"/>
+      <c r="AF26" s="593"/>
+      <c r="AG26" s="595"/>
     </row>
     <row r="27" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34"/>
@@ -18433,10 +18484,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="570" t="s">
+      <c r="AB29" s="584" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="572">
+      <c r="AC29" s="586">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -18472,11 +18523,11 @@
         <v>0</v>
       </c>
       <c r="O30" s="7"/>
-      <c r="P30" s="557">
+      <c r="P30" s="571">
         <f>SUM(P5:P29)</f>
         <v>-163726</v>
       </c>
-      <c r="Q30" s="557"/>
+      <c r="Q30" s="571"/>
       <c r="R30" s="7">
         <v>0</v>
       </c>
@@ -18490,8 +18541,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="571"/>
-      <c r="AC30" s="573"/>
+      <c r="AB30" s="585"/>
+      <c r="AC30" s="587"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -19853,21 +19904,21 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="522" t="s">
+      <c r="H64" s="532" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="523"/>
+      <c r="I64" s="533"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="524">
+      <c r="K64" s="534">
         <f>I62+L62</f>
         <v>339830.06000000006</v>
       </c>
-      <c r="L64" s="525"/>
-      <c r="M64" s="526">
+      <c r="L64" s="535"/>
+      <c r="M64" s="536">
         <f>M62+N62</f>
         <v>2936130</v>
       </c>
-      <c r="N64" s="527"/>
+      <c r="N64" s="537"/>
       <c r="O64" s="367"/>
       <c r="P64" s="367"/>
       <c r="Q64" s="367"/>
@@ -19882,40 +19933,40 @@
       <c r="AG64" s="327"/>
     </row>
     <row r="65" spans="2:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="534" t="s">
+      <c r="D65" s="544" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="534"/>
+      <c r="E65" s="544"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2702101.7199999997</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="R65" s="513">
+      <c r="R65" s="545">
         <f>R62+S62</f>
         <v>3138957.44</v>
       </c>
-      <c r="S65" s="514"/>
+      <c r="S65" s="546"/>
       <c r="U65" s="50"/>
     </row>
     <row r="66" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="515" t="s">
+      <c r="D66" s="547" t="s">
         <v>502</v>
       </c>
-      <c r="E66" s="515"/>
+      <c r="E66" s="547"/>
       <c r="F66" s="95">
         <v>-2720820.95</v>
       </c>
-      <c r="I66" s="516" t="s">
+      <c r="I66" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="517"/>
-      <c r="K66" s="518">
+      <c r="J66" s="549"/>
+      <c r="K66" s="550">
         <f>F68+F69+F70</f>
         <v>381077.48999999953</v>
       </c>
-      <c r="L66" s="519"/>
+      <c r="L66" s="551"/>
       <c r="R66" s="50"/>
       <c r="U66" s="107"/>
     </row>
@@ -19949,11 +20000,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="520">
+      <c r="K68" s="552">
         <f>-C4</f>
         <v>-255764.39</v>
       </c>
-      <c r="L68" s="521"/>
+      <c r="L68" s="553"/>
       <c r="M68" s="116"/>
       <c r="R68" s="50"/>
       <c r="S68" s="7"/>
@@ -19977,22 +20028,22 @@
       <c r="C70" s="119">
         <v>44377</v>
       </c>
-      <c r="D70" s="528" t="s">
+      <c r="D70" s="538" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="529"/>
+      <c r="E70" s="539"/>
       <c r="F70" s="120">
         <v>308642.71999999997</v>
       </c>
-      <c r="I70" s="530" t="s">
+      <c r="I70" s="540" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="531"/>
-      <c r="K70" s="532">
+      <c r="J70" s="541"/>
+      <c r="K70" s="542">
         <f>K66+K68</f>
         <v>125313.09999999951</v>
       </c>
-      <c r="L70" s="533"/>
+      <c r="L70" s="543"/>
       <c r="R70" s="50"/>
       <c r="S70" s="7"/>
       <c r="U70" s="121"/>
@@ -20008,14 +20059,14 @@
       <c r="S71" s="7"/>
     </row>
     <row r="72" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I72" s="558" t="s">
+      <c r="I72" s="572" t="s">
         <v>610</v>
       </c>
-      <c r="J72" s="559"/>
-      <c r="K72" s="562">
+      <c r="J72" s="573"/>
+      <c r="K72" s="576">
         <v>163726</v>
       </c>
-      <c r="L72" s="563"/>
+      <c r="L72" s="577"/>
       <c r="R72" s="7"/>
       <c r="S72" s="7"/>
     </row>
@@ -20024,10 +20075,10 @@
       <c r="C73" s="128"/>
       <c r="D73" s="129"/>
       <c r="E73" s="7"/>
-      <c r="I73" s="560"/>
-      <c r="J73" s="561"/>
-      <c r="K73" s="564"/>
-      <c r="L73" s="565"/>
+      <c r="I73" s="574"/>
+      <c r="J73" s="575"/>
+      <c r="K73" s="578"/>
+      <c r="L73" s="579"/>
       <c r="M73" s="2"/>
       <c r="N73" s="60"/>
       <c r="O73" s="165"/>
@@ -20079,7 +20130,7 @@
       <c r="C76" s="130"/>
       <c r="E76" s="7"/>
       <c r="M76" s="4"/>
-      <c r="AC76" s="582"/>
+      <c r="AC76" s="569"/>
       <c r="AD76" s="342"/>
       <c r="AE76" s="342"/>
       <c r="AF76" s="342"/>
@@ -20092,7 +20143,7 @@
       <c r="E77" s="7"/>
       <c r="F77" s="273"/>
       <c r="M77" s="4"/>
-      <c r="AC77" s="582"/>
+      <c r="AC77" s="569"/>
       <c r="AD77" s="342"/>
       <c r="AE77" s="342"/>
       <c r="AF77" s="342"/>
@@ -20186,22 +20237,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="AC76:AC77"/>
-    <mergeCell ref="R65:S65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="P30:Q30"/>
     <mergeCell ref="I72:J73"/>
@@ -20217,6 +20252,22 @@
     <mergeCell ref="AE23:AF23"/>
     <mergeCell ref="AE25:AF26"/>
     <mergeCell ref="AG25:AG26"/>
+    <mergeCell ref="AC76:AC77"/>
+    <mergeCell ref="R65:S65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.49" right="0.23622047244094491" top="0.47244094488188981" bottom="0.27559055118110237" header="0.70866141732283472" footer="0.31496062992125984"/>
   <pageSetup scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -21554,25 +21605,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="567" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="535" t="s">
+      <c r="C1" s="524" t="s">
         <v>503</v>
       </c>
-      <c r="D1" s="535"/>
-      <c r="E1" s="535"/>
-      <c r="F1" s="535"/>
-      <c r="G1" s="535"/>
-      <c r="H1" s="535"/>
-      <c r="I1" s="535"/>
-      <c r="J1" s="535"/>
-      <c r="K1" s="535"/>
+      <c r="D1" s="524"/>
+      <c r="E1" s="524"/>
+      <c r="F1" s="524"/>
+      <c r="G1" s="524"/>
+      <c r="H1" s="524"/>
+      <c r="I1" s="524"/>
+      <c r="J1" s="524"/>
+      <c r="K1" s="524"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="568"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -21582,27 +21633,27 @@
       <c r="L2" s="12"/>
       <c r="M2" s="3"/>
       <c r="N2" s="6"/>
-      <c r="Q2" s="566" t="s">
+      <c r="Q2" s="580" t="s">
         <v>596</v>
       </c>
-      <c r="R2" s="566"/>
-      <c r="S2" s="566"/>
-      <c r="T2" s="566"/>
-      <c r="U2" s="566"/>
-      <c r="V2" s="566"/>
+      <c r="R2" s="580"/>
+      <c r="S2" s="580"/>
+      <c r="T2" s="580"/>
+      <c r="U2" s="580"/>
+      <c r="V2" s="580"/>
     </row>
     <row r="3" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="536" t="s">
+      <c r="B3" s="525" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="537"/>
+      <c r="C3" s="526"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="538" t="s">
+      <c r="H3" s="527" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="538"/>
+      <c r="I3" s="527"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -21610,12 +21661,12 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="Q3" s="566"/>
-      <c r="R3" s="566"/>
-      <c r="S3" s="566"/>
-      <c r="T3" s="566"/>
-      <c r="U3" s="566"/>
-      <c r="V3" s="566"/>
+      <c r="Q3" s="580"/>
+      <c r="R3" s="580"/>
+      <c r="S3" s="580"/>
+      <c r="T3" s="580"/>
+      <c r="U3" s="580"/>
+      <c r="V3" s="580"/>
     </row>
     <row r="4" spans="1:23" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -21628,14 +21679,14 @@
       <c r="D4" s="23">
         <v>44353</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="528" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="529"/>
+      <c r="H4" s="530" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="531"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -21647,16 +21698,16 @@
       </c>
       <c r="O4" s="365"/>
       <c r="P4" s="29"/>
-      <c r="Q4" s="567" t="s">
+      <c r="Q4" s="581" t="s">
         <v>527</v>
       </c>
-      <c r="R4" s="568"/>
+      <c r="R4" s="582"/>
       <c r="S4" s="99"/>
-      <c r="T4" s="569" t="s">
+      <c r="T4" s="583" t="s">
         <v>567</v>
       </c>
-      <c r="U4" s="569"/>
-      <c r="V4" s="569"/>
+      <c r="U4" s="583"/>
+      <c r="V4" s="583"/>
       <c r="W4" s="99"/>
     </row>
     <row r="5" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -22655,10 +22706,10 @@
         <v>0</v>
       </c>
       <c r="S23" s="99"/>
-      <c r="T23" s="574" t="s">
+      <c r="T23" s="588" t="s">
         <v>564</v>
       </c>
-      <c r="U23" s="575"/>
+      <c r="U23" s="589"/>
       <c r="V23" s="339">
         <f>SUM(V6:V22)</f>
         <v>2323600</v>
@@ -22762,11 +22813,11 @@
         <v>138607</v>
       </c>
       <c r="S25" s="99"/>
-      <c r="T25" s="576" t="s">
+      <c r="T25" s="590" t="s">
         <v>565</v>
       </c>
-      <c r="U25" s="577"/>
-      <c r="V25" s="580">
+      <c r="U25" s="591"/>
+      <c r="V25" s="594">
         <f>R29-V23</f>
         <v>163726</v>
       </c>
@@ -22815,9 +22866,9 @@
         <v>107480</v>
       </c>
       <c r="S26" s="99"/>
-      <c r="T26" s="578"/>
-      <c r="U26" s="579"/>
-      <c r="V26" s="581"/>
+      <c r="T26" s="592"/>
+      <c r="U26" s="593"/>
+      <c r="V26" s="595"/>
       <c r="W26" s="99"/>
     </row>
     <row r="27" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -22940,10 +22991,10 @@
       </c>
       <c r="O29" s="7"/>
       <c r="P29" s="29"/>
-      <c r="Q29" s="570" t="s">
+      <c r="Q29" s="584" t="s">
         <v>562</v>
       </c>
-      <c r="R29" s="572">
+      <c r="R29" s="586">
         <f>SUM(R5:R28)</f>
         <v>2487326</v>
       </c>
@@ -22980,8 +23031,8 @@
       </c>
       <c r="O30" s="7"/>
       <c r="P30" s="373"/>
-      <c r="Q30" s="571"/>
-      <c r="R30" s="573"/>
+      <c r="Q30" s="585"/>
+      <c r="R30" s="587"/>
       <c r="S30" s="99"/>
       <c r="T30" s="99"/>
       <c r="U30" s="99"/>
@@ -23606,21 +23657,21 @@
       <c r="A50" s="60"/>
       <c r="B50" s="100"/>
       <c r="C50" s="4"/>
-      <c r="H50" s="522" t="s">
+      <c r="H50" s="532" t="s">
         <v>16</v>
       </c>
-      <c r="I50" s="523"/>
+      <c r="I50" s="533"/>
       <c r="J50" s="101"/>
-      <c r="K50" s="524">
+      <c r="K50" s="534">
         <f>I48+L48</f>
         <v>339830.06000000006</v>
       </c>
-      <c r="L50" s="525"/>
-      <c r="M50" s="526">
+      <c r="L50" s="535"/>
+      <c r="M50" s="536">
         <f>M48+N48</f>
         <v>612530</v>
       </c>
-      <c r="N50" s="527"/>
+      <c r="N50" s="537"/>
       <c r="O50" s="367"/>
       <c r="P50" s="102"/>
       <c r="Q50" s="320"/>
@@ -23632,10 +23683,10 @@
       <c r="W50" s="327"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D51" s="534" t="s">
+      <c r="D51" s="544" t="s">
         <v>17</v>
       </c>
-      <c r="E51" s="534"/>
+      <c r="E51" s="544"/>
       <c r="F51" s="103">
         <f>F48-K50-C48</f>
         <v>2702101.7199999997</v>
@@ -23644,22 +23695,22 @@
       <c r="J51" s="105"/>
     </row>
     <row r="52" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D52" s="515" t="s">
+      <c r="D52" s="547" t="s">
         <v>502</v>
       </c>
-      <c r="E52" s="515"/>
+      <c r="E52" s="547"/>
       <c r="F52" s="95">
         <v>-2720820.95</v>
       </c>
-      <c r="I52" s="516" t="s">
+      <c r="I52" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J52" s="517"/>
-      <c r="K52" s="518">
+      <c r="J52" s="549"/>
+      <c r="K52" s="550">
         <f>F54+F55+F56</f>
         <v>381077.72999999952</v>
       </c>
-      <c r="L52" s="519"/>
+      <c r="L52" s="551"/>
     </row>
     <row r="53" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D53" s="108"/>
@@ -23688,11 +23739,11 @@
         <v>21</v>
       </c>
       <c r="J54" s="115"/>
-      <c r="K54" s="520">
+      <c r="K54" s="552">
         <f>-C4</f>
         <v>-255764.39</v>
       </c>
-      <c r="L54" s="521"/>
+      <c r="L54" s="553"/>
       <c r="M54" s="116"/>
     </row>
     <row r="55" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23710,22 +23761,22 @@
       <c r="C56" s="119">
         <v>44377</v>
       </c>
-      <c r="D56" s="528" t="s">
+      <c r="D56" s="538" t="s">
         <v>24</v>
       </c>
-      <c r="E56" s="529"/>
+      <c r="E56" s="539"/>
       <c r="F56" s="120">
         <v>308642.71999999997</v>
       </c>
-      <c r="I56" s="530" t="s">
+      <c r="I56" s="540" t="s">
         <v>25</v>
       </c>
-      <c r="J56" s="531"/>
-      <c r="K56" s="532">
+      <c r="J56" s="541"/>
+      <c r="K56" s="542">
         <f>K52+K54</f>
         <v>125313.3399999995</v>
       </c>
-      <c r="L56" s="533"/>
+      <c r="L56" s="543"/>
     </row>
     <row r="57" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C57" s="122"/>
@@ -23781,7 +23832,7 @@
       <c r="C62" s="130"/>
       <c r="E62" s="7"/>
       <c r="M62" s="4"/>
-      <c r="R62" s="582"/>
+      <c r="R62" s="569"/>
       <c r="S62" s="379"/>
       <c r="T62" s="379"/>
       <c r="U62" s="379"/>
@@ -23794,7 +23845,7 @@
       <c r="E63" s="7"/>
       <c r="F63" s="273"/>
       <c r="M63" s="4"/>
-      <c r="R63" s="582"/>
+      <c r="R63" s="569"/>
       <c r="S63" s="379"/>
       <c r="T63" s="379"/>
       <c r="U63" s="379"/>
@@ -23871,23 +23922,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Q2:V3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="T25:U26"/>
-    <mergeCell ref="V25:V26"/>
-    <mergeCell ref="Q29:Q30"/>
-    <mergeCell ref="R29:R30"/>
     <mergeCell ref="R62:R63"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="D52:E52"/>
@@ -23897,6 +23931,23 @@
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="I56:J56"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="T25:U26"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="Q29:Q30"/>
+    <mergeCell ref="R29:R30"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="Q2:V3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="T4:V4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -23915,7 +23966,7 @@
       <pane xSplit="5" ySplit="4" topLeftCell="F62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K77" sqref="K77:L78"/>
+      <selection pane="bottomRight" activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -23950,20 +24001,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="567" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="535" t="s">
+      <c r="C1" s="524" t="s">
         <v>720</v>
       </c>
-      <c r="D1" s="535"/>
-      <c r="E1" s="535"/>
-      <c r="F1" s="535"/>
-      <c r="G1" s="535"/>
-      <c r="H1" s="535"/>
-      <c r="I1" s="535"/>
-      <c r="J1" s="535"/>
-      <c r="K1" s="535"/>
+      <c r="D1" s="524"/>
+      <c r="E1" s="524"/>
+      <c r="F1" s="524"/>
+      <c r="G1" s="524"/>
+      <c r="H1" s="524"/>
+      <c r="I1" s="524"/>
+      <c r="J1" s="524"/>
+      <c r="K1" s="524"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -23973,7 +24024,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="568"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -23992,27 +24043,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="566" t="s">
+      <c r="AB2" s="580" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="566"/>
-      <c r="AD2" s="566"/>
-      <c r="AE2" s="566"/>
-      <c r="AF2" s="566"/>
-      <c r="AG2" s="566"/>
+      <c r="AC2" s="580"/>
+      <c r="AD2" s="580"/>
+      <c r="AE2" s="580"/>
+      <c r="AF2" s="580"/>
+      <c r="AG2" s="580"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="536" t="s">
+      <c r="B3" s="525" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="537"/>
+      <c r="C3" s="526"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="538" t="s">
+      <c r="H3" s="527" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="538"/>
+      <c r="I3" s="527"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -24020,13 +24071,13 @@
         <v>4</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="P3" s="585" t="s">
+      <c r="P3" s="618" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="587" t="s">
+      <c r="Q3" s="620" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="588"/>
+      <c r="S3" s="621"/>
       <c r="W3" s="213" t="s">
         <v>54</v>
       </c>
@@ -24036,12 +24087,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="566"/>
-      <c r="AC3" s="566"/>
-      <c r="AD3" s="566"/>
-      <c r="AE3" s="566"/>
-      <c r="AF3" s="566"/>
-      <c r="AG3" s="566"/>
+      <c r="AB3" s="580"/>
+      <c r="AC3" s="580"/>
+      <c r="AD3" s="580"/>
+      <c r="AE3" s="580"/>
+      <c r="AF3" s="580"/>
+      <c r="AG3" s="580"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -24054,14 +24105,14 @@
       <c r="D4" s="23">
         <v>44377</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="528" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="586" t="s">
+      <c r="F4" s="529"/>
+      <c r="H4" s="619" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="531"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -24072,10 +24123,10 @@
         <v>10</v>
       </c>
       <c r="O4" s="365"/>
-      <c r="P4" s="585"/>
-      <c r="Q4" s="587"/>
+      <c r="P4" s="618"/>
+      <c r="Q4" s="620"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="588"/>
+      <c r="S4" s="621"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -24087,16 +24138,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="567" t="s">
+      <c r="AB4" s="581" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="568"/>
+      <c r="AC4" s="582"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="569" t="s">
+      <c r="AE4" s="583" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="569"/>
-      <c r="AG4" s="569"/>
+      <c r="AF4" s="583"/>
+      <c r="AG4" s="583"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -25533,10 +25584,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="574" t="s">
+      <c r="AE23" s="588" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="575"/>
+      <c r="AF23" s="589"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -25668,11 +25719,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="576" t="s">
+      <c r="AE25" s="590" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="577"/>
-      <c r="AG25" s="580">
+      <c r="AF25" s="591"/>
+      <c r="AG25" s="594">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -25741,9 +25792,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="578"/>
-      <c r="AF26" s="579"/>
-      <c r="AG26" s="581"/>
+      <c r="AE26" s="592"/>
+      <c r="AF26" s="593"/>
+      <c r="AG26" s="595"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -25942,10 +25993,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="570" t="s">
+      <c r="AB29" s="584" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="572">
+      <c r="AC29" s="586">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -26008,8 +26059,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="571"/>
-      <c r="AC30" s="573"/>
+      <c r="AB30" s="585"/>
+      <c r="AC30" s="587"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -26502,11 +26553,11 @@
       <c r="J39" s="233"/>
       <c r="K39" s="361"/>
       <c r="L39" s="357"/>
-      <c r="M39" s="597">
+      <c r="M39" s="613">
         <f>SUM(M5:M38)</f>
         <v>3989472.22</v>
       </c>
-      <c r="N39" s="599">
+      <c r="N39" s="615">
         <f>SUM(N5:N38)</f>
         <v>689220.5</v>
       </c>
@@ -26555,8 +26606,8 @@
         <f>1145.91+398.99+423.94+498.99+398.99</f>
         <v>2866.8199999999997</v>
       </c>
-      <c r="M40" s="598"/>
-      <c r="N40" s="600"/>
+      <c r="M40" s="614"/>
+      <c r="N40" s="616"/>
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -26749,10 +26800,10 @@
       <c r="L44" s="358">
         <v>73526</v>
       </c>
-      <c r="M44" s="601" t="s">
+      <c r="M44" s="617" t="s">
         <v>567</v>
       </c>
-      <c r="N44" s="601"/>
+      <c r="N44" s="617"/>
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -27340,7 +27391,7 @@
       <c r="L57" s="458">
         <v>7482</v>
       </c>
-      <c r="M57" s="589">
+      <c r="M57" s="605">
         <f>SUM(M45:M56)</f>
         <v>3606750</v>
       </c>
@@ -27380,7 +27431,7 @@
       <c r="L58" s="458">
         <v>986</v>
       </c>
-      <c r="M58" s="590"/>
+      <c r="M58" s="606"/>
       <c r="N58" s="476"/>
       <c r="O58" s="7"/>
       <c r="P58" s="7"/>
@@ -27455,10 +27506,10 @@
         <f>1033.33+165.33</f>
         <v>1198.6599999999999</v>
       </c>
-      <c r="M60" s="591" t="s">
+      <c r="M60" s="607" t="s">
         <v>719</v>
       </c>
-      <c r="N60" s="592"/>
+      <c r="N60" s="608"/>
       <c r="O60" s="7"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -27531,11 +27582,11 @@
       <c r="L62" s="458">
         <v>22595.71</v>
       </c>
-      <c r="M62" s="593">
+      <c r="M62" s="609">
         <f>M57-M39</f>
         <v>-382722.2200000002</v>
       </c>
-      <c r="N62" s="594"/>
+      <c r="N62" s="610"/>
       <c r="O62" s="7"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
@@ -27571,8 +27622,8 @@
       <c r="L63" s="458">
         <v>1064</v>
       </c>
-      <c r="M63" s="595"/>
-      <c r="N63" s="596"/>
+      <c r="M63" s="611"/>
+      <c r="N63" s="612"/>
       <c r="O63" s="7"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
@@ -27762,16 +27813,16 @@
       <c r="A69" s="60"/>
       <c r="B69" s="100"/>
       <c r="C69" s="4"/>
-      <c r="H69" s="522" t="s">
+      <c r="H69" s="532" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="523"/>
+      <c r="I69" s="533"/>
       <c r="J69" s="101"/>
-      <c r="K69" s="524">
+      <c r="K69" s="534">
         <f>I67+L67</f>
         <v>587206.12</v>
       </c>
-      <c r="L69" s="525"/>
+      <c r="L69" s="535"/>
       <c r="M69" s="471"/>
       <c r="N69" s="472"/>
       <c r="O69" s="367"/>
@@ -27788,40 +27839,40 @@
       <c r="AG69" s="327"/>
     </row>
     <row r="70" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="534" t="s">
+      <c r="D70" s="544" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="534"/>
+      <c r="E70" s="544"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
         <v>3436910.52</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="513">
+      <c r="R70" s="545">
         <f>R67+S67</f>
         <v>10503773.959999999</v>
       </c>
-      <c r="S70" s="514"/>
+      <c r="S70" s="546"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="515" t="s">
+      <c r="D71" s="547" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="515"/>
+      <c r="E71" s="547"/>
       <c r="F71" s="95">
         <v>-3290264.27</v>
       </c>
-      <c r="I71" s="516" t="s">
+      <c r="I71" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="517"/>
-      <c r="K71" s="518">
+      <c r="J71" s="549"/>
+      <c r="K71" s="550">
         <f>F73+F74+F75</f>
         <v>426565.1</v>
       </c>
-      <c r="L71" s="519"/>
+      <c r="L71" s="551"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -27855,11 +27906,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="520">
+      <c r="K73" s="552">
         <f>-C4</f>
         <v>-308642.71999999997</v>
       </c>
-      <c r="L73" s="602"/>
+      <c r="L73" s="596"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -27882,22 +27933,22 @@
       <c r="C75" s="119">
         <v>44410</v>
       </c>
-      <c r="D75" s="528" t="s">
+      <c r="D75" s="538" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="529"/>
+      <c r="E75" s="539"/>
       <c r="F75" s="120">
         <v>250140.85</v>
       </c>
-      <c r="I75" s="530" t="s">
+      <c r="I75" s="540" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="531"/>
-      <c r="K75" s="532">
+      <c r="J75" s="541"/>
+      <c r="K75" s="542">
         <f>K71+K73</f>
         <v>117922.38</v>
       </c>
-      <c r="L75" s="532"/>
+      <c r="L75" s="542"/>
       <c r="R75" s="50"/>
       <c r="S75" s="7"/>
       <c r="U75" s="121"/>
@@ -27912,14 +27963,14 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="603" t="s">
+      <c r="I77" s="597" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="604"/>
-      <c r="K77" s="607">
+      <c r="J77" s="598"/>
+      <c r="K77" s="601">
         <v>-383122.22</v>
       </c>
-      <c r="L77" s="608"/>
+      <c r="L77" s="602"/>
       <c r="R77" s="7"/>
       <c r="S77" s="7"/>
     </row>
@@ -27928,10 +27979,10 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="605"/>
-      <c r="J78" s="606"/>
-      <c r="K78" s="609"/>
-      <c r="L78" s="610"/>
+      <c r="I78" s="599"/>
+      <c r="J78" s="600"/>
+      <c r="K78" s="603"/>
+      <c r="L78" s="604"/>
       <c r="M78" s="2"/>
       <c r="N78" s="60"/>
       <c r="O78" s="165"/>
@@ -27983,7 +28034,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="582"/>
+      <c r="AC81" s="569"/>
       <c r="AD81" s="440"/>
       <c r="AE81" s="440"/>
       <c r="AF81" s="440"/>
@@ -27996,7 +28047,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="582"/>
+      <c r="AC82" s="569"/>
       <c r="AD82" s="440"/>
       <c r="AE82" s="440"/>
       <c r="AF82" s="440"/>
@@ -28090,13 +28141,21 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="AC81:AC82"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="I77:J78"/>
-    <mergeCell ref="K77:L78"/>
+    <mergeCell ref="AG25:AG26"/>
+    <mergeCell ref="AB29:AB30"/>
+    <mergeCell ref="AC29:AC30"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="AB2:AG3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="S3:S4"/>
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="I71:J71"/>
     <mergeCell ref="K71:L71"/>
@@ -28112,21 +28171,13 @@
     <mergeCell ref="M39:M40"/>
     <mergeCell ref="N39:N40"/>
     <mergeCell ref="M44:N44"/>
-    <mergeCell ref="AG25:AG26"/>
-    <mergeCell ref="AB29:AB30"/>
-    <mergeCell ref="AC29:AC30"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="AB2:AG3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="AC81:AC82"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="I77:J78"/>
+    <mergeCell ref="K77:L78"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.27559055118110237" top="0.27559055118110237" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -29773,8 +29824,8 @@
   </sheetPr>
   <dimension ref="A1:AG97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N72" sqref="N72"/>
+    <sheetView topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -29809,20 +29860,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="583" t="s">
+      <c r="B1" s="567" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="535" t="s">
+      <c r="C1" s="524" t="s">
         <v>721</v>
       </c>
-      <c r="D1" s="535"/>
-      <c r="E1" s="535"/>
-      <c r="F1" s="535"/>
-      <c r="G1" s="535"/>
-      <c r="H1" s="535"/>
-      <c r="I1" s="535"/>
-      <c r="J1" s="535"/>
-      <c r="K1" s="535"/>
+      <c r="D1" s="524"/>
+      <c r="E1" s="524"/>
+      <c r="F1" s="524"/>
+      <c r="G1" s="524"/>
+      <c r="H1" s="524"/>
+      <c r="I1" s="524"/>
+      <c r="J1" s="524"/>
+      <c r="K1" s="524"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="W1" s="209"/>
@@ -29832,7 +29883,7 @@
       <c r="Y1" s="206"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="584"/>
+      <c r="B2" s="568"/>
       <c r="C2" s="8"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
@@ -29851,27 +29902,27 @@
       <c r="Y2" s="216" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="566" t="s">
+      <c r="AB2" s="580" t="s">
         <v>596</v>
       </c>
-      <c r="AC2" s="566"/>
-      <c r="AD2" s="566"/>
-      <c r="AE2" s="566"/>
-      <c r="AF2" s="566"/>
-      <c r="AG2" s="566"/>
+      <c r="AC2" s="580"/>
+      <c r="AD2" s="580"/>
+      <c r="AE2" s="580"/>
+      <c r="AF2" s="580"/>
+      <c r="AG2" s="580"/>
     </row>
     <row r="3" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="536" t="s">
+      <c r="B3" s="525" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="537"/>
+      <c r="C3" s="526"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="538" t="s">
+      <c r="H3" s="527" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="538"/>
+      <c r="I3" s="527"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -29882,13 +29933,13 @@
       <c r="O3" s="366" t="s">
         <v>753</v>
       </c>
-      <c r="P3" s="585" t="s">
+      <c r="P3" s="618" t="s">
         <v>663</v>
       </c>
-      <c r="Q3" s="587" t="s">
+      <c r="Q3" s="620" t="s">
         <v>665</v>
       </c>
-      <c r="S3" s="588"/>
+      <c r="S3" s="621"/>
       <c r="W3" s="213" t="s">
         <v>54</v>
       </c>
@@ -29898,12 +29949,12 @@
       <c r="Y3" s="198">
         <v>2000</v>
       </c>
-      <c r="AB3" s="566"/>
-      <c r="AC3" s="566"/>
-      <c r="AD3" s="566"/>
-      <c r="AE3" s="566"/>
-      <c r="AF3" s="566"/>
-      <c r="AG3" s="566"/>
+      <c r="AB3" s="580"/>
+      <c r="AC3" s="580"/>
+      <c r="AD3" s="580"/>
+      <c r="AE3" s="580"/>
+      <c r="AF3" s="580"/>
+      <c r="AG3" s="580"/>
     </row>
     <row r="4" spans="1:33" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
@@ -29916,14 +29967,14 @@
       <c r="D4" s="23">
         <v>44411</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="528" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="586" t="s">
+      <c r="F4" s="529"/>
+      <c r="H4" s="619" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="531"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -29934,10 +29985,10 @@
         <v>11</v>
       </c>
       <c r="O4" s="99"/>
-      <c r="P4" s="585"/>
-      <c r="Q4" s="587"/>
+      <c r="P4" s="618"/>
+      <c r="Q4" s="620"/>
       <c r="R4" s="30"/>
-      <c r="S4" s="588"/>
+      <c r="S4" s="621"/>
       <c r="T4" s="30"/>
       <c r="U4" s="30"/>
       <c r="W4" s="213" t="s">
@@ -29949,16 +30000,16 @@
       <c r="Y4" s="217">
         <v>2000</v>
       </c>
-      <c r="AB4" s="567" t="s">
+      <c r="AB4" s="581" t="s">
         <v>527</v>
       </c>
-      <c r="AC4" s="568"/>
+      <c r="AC4" s="582"/>
       <c r="AD4" s="99"/>
-      <c r="AE4" s="569" t="s">
+      <c r="AE4" s="583" t="s">
         <v>567</v>
       </c>
-      <c r="AF4" s="569"/>
-      <c r="AG4" s="569"/>
+      <c r="AF4" s="583"/>
+      <c r="AG4" s="583"/>
     </row>
     <row r="5" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
@@ -31446,10 +31497,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="99"/>
-      <c r="AE23" s="574" t="s">
+      <c r="AE23" s="588" t="s">
         <v>564</v>
       </c>
-      <c r="AF23" s="575"/>
+      <c r="AF23" s="589"/>
       <c r="AG23" s="339">
         <f>SUM(AG6:AG22)</f>
         <v>2323600</v>
@@ -31589,11 +31640,11 @@
         <v>138607</v>
       </c>
       <c r="AD25" s="99"/>
-      <c r="AE25" s="576" t="s">
+      <c r="AE25" s="590" t="s">
         <v>565</v>
       </c>
-      <c r="AF25" s="577"/>
-      <c r="AG25" s="580">
+      <c r="AF25" s="591"/>
+      <c r="AG25" s="594">
         <f>AC29-AG23</f>
         <v>163726</v>
       </c>
@@ -31665,9 +31716,9 @@
         <v>107480</v>
       </c>
       <c r="AD26" s="99"/>
-      <c r="AE26" s="578"/>
-      <c r="AF26" s="579"/>
-      <c r="AG26" s="581"/>
+      <c r="AE26" s="592"/>
+      <c r="AF26" s="593"/>
+      <c r="AG26" s="595"/>
     </row>
     <row r="27" spans="1:33" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34"/>
@@ -31877,10 +31928,10 @@
       </c>
       <c r="X29" s="220"/>
       <c r="Y29" s="218"/>
-      <c r="AB29" s="570" t="s">
+      <c r="AB29" s="584" t="s">
         <v>562</v>
       </c>
-      <c r="AC29" s="572">
+      <c r="AC29" s="586">
         <f>SUM(AC5:AC28)</f>
         <v>2487326</v>
       </c>
@@ -31945,8 +31996,8 @@
       </c>
       <c r="X30" s="221"/>
       <c r="Y30" s="207"/>
-      <c r="AB30" s="571"/>
-      <c r="AC30" s="573"/>
+      <c r="AB30" s="585"/>
+      <c r="AC30" s="587"/>
       <c r="AD30" s="99"/>
       <c r="AE30" s="99"/>
       <c r="AF30" s="99"/>
@@ -32137,7 +32188,7 @@
         <v>10815.4</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:33" ht="31.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="34"/>
       <c r="B34" s="134"/>
       <c r="C34" s="36">
@@ -32153,9 +32204,15 @@
       <c r="I34" s="38">
         <v>0</v>
       </c>
-      <c r="J34" s="233"/>
-      <c r="K34" s="454"/>
-      <c r="L34" s="360"/>
+      <c r="J34" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K34" s="454" t="s">
+        <v>550</v>
+      </c>
+      <c r="L34" s="360">
+        <v>5046</v>
+      </c>
       <c r="M34" s="444">
         <v>0</v>
       </c>
@@ -32169,11 +32226,11 @@
       </c>
       <c r="R34" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5046</v>
       </c>
       <c r="S34" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5046</v>
       </c>
       <c r="T34" s="48"/>
       <c r="W34" s="213" t="s">
@@ -32206,9 +32263,15 @@
       <c r="I35" s="38">
         <v>0</v>
       </c>
-      <c r="J35" s="233"/>
-      <c r="K35" s="144"/>
-      <c r="L35" s="358"/>
+      <c r="J35" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K35" s="144" t="s">
+        <v>839</v>
+      </c>
+      <c r="L35" s="358">
+        <v>798</v>
+      </c>
       <c r="M35" s="444">
         <v>0</v>
       </c>
@@ -32222,11 +32285,11 @@
       </c>
       <c r="R35" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>798</v>
       </c>
       <c r="S35" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>798</v>
       </c>
       <c r="T35" s="48"/>
       <c r="W35" s="213" t="s">
@@ -32244,7 +32307,7 @@
       <c r="B36" s="146">
         <v>44412</v>
       </c>
-      <c r="C36" s="71">
+      <c r="C36" s="225">
         <v>14693.64</v>
       </c>
       <c r="D36" s="242" t="s">
@@ -32259,9 +32322,16 @@
       <c r="I36" s="38">
         <v>0</v>
       </c>
-      <c r="J36" s="233"/>
-      <c r="K36" s="359"/>
-      <c r="L36" s="360"/>
+      <c r="J36" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K36" s="359" t="s">
+        <v>827</v>
+      </c>
+      <c r="L36" s="360">
+        <f>3244.52+5324.4</f>
+        <v>8568.92</v>
+      </c>
       <c r="M36" s="444">
         <v>0</v>
       </c>
@@ -32275,7 +32345,7 @@
       </c>
       <c r="R36" s="7">
         <f t="shared" si="1"/>
-        <v>14693.64</v>
+        <v>23262.559999999998</v>
       </c>
       <c r="S36" s="6">
         <v>0</v>
@@ -32296,7 +32366,7 @@
       <c r="B37" s="146">
         <v>44415</v>
       </c>
-      <c r="C37" s="71">
+      <c r="C37" s="225">
         <v>25517.34</v>
       </c>
       <c r="D37" s="242" t="s">
@@ -32311,9 +32381,16 @@
       <c r="I37" s="38">
         <v>0</v>
       </c>
-      <c r="J37" s="233"/>
-      <c r="K37" s="144"/>
-      <c r="L37" s="358"/>
+      <c r="J37" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K37" s="144" t="s">
+        <v>582</v>
+      </c>
+      <c r="L37" s="358">
+        <f>198.99+352.4+1721.05</f>
+        <v>2272.44</v>
+      </c>
       <c r="M37" s="444">
         <v>0</v>
       </c>
@@ -32325,7 +32402,7 @@
       <c r="Q37" s="449"/>
       <c r="R37" s="7">
         <f t="shared" si="1"/>
-        <v>25517.34</v>
+        <v>27789.78</v>
       </c>
       <c r="S37" s="6">
         <v>0</v>
@@ -32353,7 +32430,7 @@
       <c r="B38" s="146">
         <v>44419</v>
       </c>
-      <c r="C38" s="71">
+      <c r="C38" s="225">
         <v>23707.279999999999</v>
       </c>
       <c r="D38" s="242" t="s">
@@ -32368,9 +32445,15 @@
       <c r="I38" s="38">
         <v>0</v>
       </c>
-      <c r="J38" s="233"/>
-      <c r="K38" s="144"/>
-      <c r="L38" s="358"/>
+      <c r="J38" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K38" s="144" t="s">
+        <v>370</v>
+      </c>
+      <c r="L38" s="358">
+        <v>549</v>
+      </c>
       <c r="M38" s="444">
         <v>0</v>
       </c>
@@ -32382,7 +32465,7 @@
       <c r="Q38" s="450"/>
       <c r="R38" s="7">
         <f t="shared" si="1"/>
-        <v>23707.279999999999</v>
+        <v>24256.28</v>
       </c>
       <c r="S38" s="6">
         <v>0</v>
@@ -32404,10 +32487,10 @@
     </row>
     <row r="39" spans="1:33" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="34"/>
-      <c r="B39" s="629">
+      <c r="B39" s="513">
         <v>44425</v>
       </c>
-      <c r="C39" s="71">
+      <c r="C39" s="225">
         <v>20092.59</v>
       </c>
       <c r="D39" s="242" t="s">
@@ -32418,14 +32501,20 @@
       <c r="G39" s="137"/>
       <c r="H39" s="138"/>
       <c r="I39" s="69"/>
-      <c r="J39" s="233"/>
-      <c r="K39" s="361"/>
-      <c r="L39" s="357"/>
-      <c r="M39" s="597">
+      <c r="J39" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K39" s="361" t="s">
+        <v>828</v>
+      </c>
+      <c r="L39" s="357">
+        <v>11500</v>
+      </c>
+      <c r="M39" s="613">
         <f>SUM(M5:M38)</f>
         <v>2842451</v>
       </c>
-      <c r="N39" s="599">
+      <c r="N39" s="615">
         <f>SUM(N5:N38)</f>
         <v>271503</v>
       </c>
@@ -32434,7 +32523,7 @@
       <c r="Q39" s="7"/>
       <c r="R39" s="7">
         <f>SUM(R5:R38)</f>
-        <v>3640891.4</v>
+        <v>3658125.76</v>
       </c>
       <c r="T39" s="48"/>
       <c r="W39" s="213" t="s">
@@ -32453,10 +32542,10 @@
     </row>
     <row r="40" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="34"/>
-      <c r="B40" s="629">
+      <c r="B40" s="513">
         <v>44427</v>
       </c>
-      <c r="C40" s="71">
+      <c r="C40" s="225">
         <v>11142.75</v>
       </c>
       <c r="D40" s="242" t="s">
@@ -32467,11 +32556,17 @@
       <c r="G40" s="137"/>
       <c r="H40" s="138"/>
       <c r="I40" s="69"/>
-      <c r="J40" s="233"/>
-      <c r="K40" s="144"/>
-      <c r="L40" s="357"/>
-      <c r="M40" s="598"/>
-      <c r="N40" s="600"/>
+      <c r="J40" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K40" s="144" t="s">
+        <v>829</v>
+      </c>
+      <c r="L40" s="357">
+        <v>20880</v>
+      </c>
+      <c r="M40" s="614"/>
+      <c r="N40" s="616"/>
       <c r="O40" s="392"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -32496,10 +32591,10 @@
     </row>
     <row r="41" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="34"/>
-      <c r="B41" s="629">
+      <c r="B41" s="513">
         <v>44428</v>
       </c>
-      <c r="C41" s="71">
+      <c r="C41" s="225">
         <v>24621.96</v>
       </c>
       <c r="D41" s="242" t="s">
@@ -32510,9 +32605,16 @@
       <c r="G41" s="137"/>
       <c r="H41" s="138"/>
       <c r="I41" s="69"/>
-      <c r="J41" s="233"/>
-      <c r="K41" s="144"/>
-      <c r="L41" s="357"/>
+      <c r="J41" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K41" s="144" t="s">
+        <v>548</v>
+      </c>
+      <c r="L41" s="357">
+        <f>9720+9720+9885+9720</f>
+        <v>39045</v>
+      </c>
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="392"/>
@@ -32540,10 +32642,10 @@
     </row>
     <row r="42" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="34"/>
-      <c r="B42" s="630">
+      <c r="B42" s="514">
         <v>44434</v>
       </c>
-      <c r="C42" s="71">
+      <c r="C42" s="225">
         <v>23223.96</v>
       </c>
       <c r="D42" s="242" t="s">
@@ -32554,9 +32656,15 @@
       <c r="G42" s="137"/>
       <c r="H42" s="138"/>
       <c r="I42" s="69"/>
-      <c r="J42" s="233"/>
-      <c r="K42" s="144"/>
-      <c r="L42" s="357"/>
+      <c r="J42" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K42" s="144" t="s">
+        <v>830</v>
+      </c>
+      <c r="L42" s="357">
+        <v>5220</v>
+      </c>
       <c r="M42" s="7"/>
       <c r="N42" s="7"/>
       <c r="O42" s="392"/>
@@ -32584,7 +32692,7 @@
       <c r="B43" s="146">
         <v>44435</v>
       </c>
-      <c r="C43" s="71">
+      <c r="C43" s="225">
         <v>12717.12</v>
       </c>
       <c r="D43" s="242" t="s">
@@ -32595,9 +32703,16 @@
       <c r="G43" s="137"/>
       <c r="H43" s="138"/>
       <c r="I43" s="69"/>
-      <c r="J43" s="233"/>
-      <c r="K43" s="144"/>
-      <c r="L43" s="357"/>
+      <c r="J43" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K43" s="144" t="s">
+        <v>132</v>
+      </c>
+      <c r="L43" s="357">
+        <f>3678.2+1492.43+1055.91</f>
+        <v>6226.54</v>
+      </c>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
       <c r="O43" s="392"/>
@@ -32625,7 +32740,7 @@
       <c r="B44" s="146">
         <v>44436</v>
       </c>
-      <c r="C44" s="71">
+      <c r="C44" s="225">
         <v>9197.25</v>
       </c>
       <c r="D44" s="242" t="s">
@@ -32636,13 +32751,19 @@
       <c r="G44" s="137"/>
       <c r="H44" s="138"/>
       <c r="I44" s="69"/>
-      <c r="J44" s="233"/>
-      <c r="K44" s="228"/>
-      <c r="L44" s="358"/>
-      <c r="M44" s="601" t="s">
+      <c r="J44" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K44" s="228" t="s">
+        <v>136</v>
+      </c>
+      <c r="L44" s="358">
+        <v>986</v>
+      </c>
+      <c r="M44" s="617" t="s">
         <v>567</v>
       </c>
-      <c r="N44" s="601"/>
+      <c r="N44" s="617"/>
       <c r="O44" s="392"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -32680,10 +32801,16 @@
       <c r="G45" s="137"/>
       <c r="H45" s="138"/>
       <c r="I45" s="69"/>
-      <c r="J45" s="233"/>
-      <c r="K45" s="228"/>
-      <c r="L45" s="358"/>
-      <c r="M45" s="631">
+      <c r="J45" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K45" s="362" t="s">
+        <v>831</v>
+      </c>
+      <c r="L45" s="66">
+        <v>55555.55</v>
+      </c>
+      <c r="M45" s="515">
         <v>330120</v>
       </c>
       <c r="N45" s="473">
@@ -32716,10 +32843,16 @@
       <c r="G46" s="137"/>
       <c r="H46" s="138"/>
       <c r="I46" s="69"/>
-      <c r="J46" s="233"/>
-      <c r="K46" s="168"/>
-      <c r="L46" s="66"/>
-      <c r="M46" s="632">
+      <c r="J46" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K46" s="459" t="s">
+        <v>832</v>
+      </c>
+      <c r="L46" s="458">
+        <v>12148.56</v>
+      </c>
+      <c r="M46" s="516">
         <v>300000</v>
       </c>
       <c r="N46" s="473">
@@ -32752,10 +32885,16 @@
       <c r="G47" s="137"/>
       <c r="H47" s="138"/>
       <c r="I47" s="69"/>
-      <c r="J47" s="233"/>
-      <c r="K47" s="144"/>
-      <c r="L47" s="66"/>
-      <c r="M47" s="632">
+      <c r="J47" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K47" s="144" t="s">
+        <v>833</v>
+      </c>
+      <c r="L47" s="66">
+        <v>2080</v>
+      </c>
+      <c r="M47" s="516">
         <v>324890</v>
       </c>
       <c r="N47" s="473">
@@ -32785,10 +32924,16 @@
       <c r="G48" s="137"/>
       <c r="H48" s="138"/>
       <c r="I48" s="69"/>
-      <c r="J48" s="233"/>
-      <c r="K48" s="144"/>
-      <c r="L48" s="66"/>
-      <c r="M48" s="633">
+      <c r="J48" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K48" s="144" t="s">
+        <v>834</v>
+      </c>
+      <c r="L48" s="66">
+        <v>67711</v>
+      </c>
+      <c r="M48" s="517">
         <v>159870</v>
       </c>
       <c r="N48" s="474">
@@ -32818,10 +32963,16 @@
       <c r="G49" s="137"/>
       <c r="H49" s="138"/>
       <c r="I49" s="69"/>
-      <c r="J49" s="233"/>
-      <c r="K49" s="144"/>
-      <c r="L49" s="66"/>
-      <c r="M49" s="634">
+      <c r="J49" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K49" s="144" t="s">
+        <v>225</v>
+      </c>
+      <c r="L49" s="66">
+        <v>10000</v>
+      </c>
+      <c r="M49" s="518">
         <v>384800</v>
       </c>
       <c r="N49" s="474">
@@ -32852,10 +33003,16 @@
       <c r="G50" s="137"/>
       <c r="H50" s="138"/>
       <c r="I50" s="69"/>
-      <c r="J50" s="233"/>
-      <c r="K50" s="144"/>
-      <c r="L50" s="66"/>
-      <c r="M50" s="634">
+      <c r="J50" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K50" s="144" t="s">
+        <v>835</v>
+      </c>
+      <c r="L50" s="66">
+        <v>8928.69</v>
+      </c>
+      <c r="M50" s="518">
         <v>177370</v>
       </c>
       <c r="N50" s="473">
@@ -32886,10 +33043,17 @@
       <c r="G51" s="137"/>
       <c r="H51" s="138"/>
       <c r="I51" s="69"/>
-      <c r="J51" s="233"/>
-      <c r="K51" s="144"/>
-      <c r="L51" s="66"/>
-      <c r="M51" s="635">
+      <c r="J51" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K51" s="144" t="s">
+        <v>836</v>
+      </c>
+      <c r="L51" s="66">
+        <f>2990+478.4</f>
+        <v>3468.4</v>
+      </c>
+      <c r="M51" s="519">
         <v>375140</v>
       </c>
       <c r="N51" s="473">
@@ -32922,10 +33086,14 @@
       <c r="G52" s="137"/>
       <c r="H52" s="138"/>
       <c r="I52" s="69"/>
-      <c r="J52" s="233"/>
-      <c r="K52" s="144"/>
-      <c r="L52" s="66"/>
-      <c r="M52" s="634">
+      <c r="J52" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K52" s="362"/>
+      <c r="L52" s="66">
+        <v>3016</v>
+      </c>
+      <c r="M52" s="518">
         <v>100000</v>
       </c>
       <c r="N52" s="473">
@@ -32960,10 +33128,14 @@
       <c r="I53" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="J53" s="233"/>
-      <c r="K53" s="168"/>
-      <c r="L53" s="66"/>
-      <c r="M53" s="634">
+      <c r="J53" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K53" s="656"/>
+      <c r="L53" s="66">
+        <v>3480</v>
+      </c>
+      <c r="M53" s="518">
         <v>77570</v>
       </c>
       <c r="N53" s="473">
@@ -32996,10 +33168,14 @@
       <c r="G54" s="137"/>
       <c r="H54" s="138"/>
       <c r="I54" s="69"/>
-      <c r="J54" s="233"/>
-      <c r="K54" s="457"/>
-      <c r="L54" s="66"/>
-      <c r="M54" s="634">
+      <c r="J54" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K54" s="657"/>
+      <c r="L54" s="66">
+        <v>31064</v>
+      </c>
+      <c r="M54" s="518">
         <v>95470</v>
       </c>
       <c r="N54" s="473">
@@ -33032,10 +33208,14 @@
       <c r="G55" s="137"/>
       <c r="H55" s="138"/>
       <c r="I55" s="69"/>
-      <c r="J55" s="233"/>
-      <c r="K55" s="144"/>
-      <c r="L55" s="66"/>
-      <c r="M55" s="636">
+      <c r="J55" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K55" s="362"/>
+      <c r="L55" s="66">
+        <v>5046</v>
+      </c>
+      <c r="M55" s="520">
         <v>162900</v>
       </c>
       <c r="N55" s="475">
@@ -33067,10 +33247,16 @@
       <c r="G56" s="137"/>
       <c r="H56" s="145"/>
       <c r="I56" s="80"/>
-      <c r="J56" s="233"/>
-      <c r="K56" s="359"/>
-      <c r="L56" s="458"/>
-      <c r="M56" s="637">
+      <c r="J56" s="233" t="s">
+        <v>826</v>
+      </c>
+      <c r="K56" s="359" t="s">
+        <v>834</v>
+      </c>
+      <c r="L56" s="458">
+        <v>11205.93</v>
+      </c>
+      <c r="M56" s="521">
         <v>316990</v>
       </c>
       <c r="N56" s="473">
@@ -33102,9 +33288,15 @@
       <c r="G57" s="137"/>
       <c r="H57" s="145"/>
       <c r="I57" s="80"/>
-      <c r="J57" s="325"/>
-      <c r="K57" s="359"/>
-      <c r="L57" s="458"/>
+      <c r="J57" s="325" t="s">
+        <v>826</v>
+      </c>
+      <c r="K57" s="359" t="s">
+        <v>837</v>
+      </c>
+      <c r="L57" s="458">
+        <v>1229</v>
+      </c>
       <c r="M57" s="477">
         <v>0</v>
       </c>
@@ -33135,10 +33327,17 @@
       <c r="G58" s="137"/>
       <c r="H58" s="145"/>
       <c r="I58" s="80"/>
-      <c r="J58" s="325"/>
-      <c r="K58" s="457"/>
-      <c r="L58" s="458"/>
-      <c r="M58" s="648">
+      <c r="J58" s="325" t="s">
+        <v>826</v>
+      </c>
+      <c r="K58" s="462" t="s">
+        <v>838</v>
+      </c>
+      <c r="L58" s="458">
+        <f>968.75+155</f>
+        <v>1123.75</v>
+      </c>
+      <c r="M58" s="630">
         <f ca="1">SUM(M45:M58)</f>
         <v>2805120</v>
       </c>
@@ -33169,10 +33368,14 @@
       <c r="G59" s="137"/>
       <c r="H59" s="145"/>
       <c r="I59" s="80"/>
-      <c r="J59" s="325"/>
-      <c r="K59" s="359"/>
-      <c r="L59" s="458"/>
-      <c r="M59" s="649"/>
+      <c r="J59" s="325" t="s">
+        <v>826</v>
+      </c>
+      <c r="K59" s="459"/>
+      <c r="L59" s="458">
+        <v>1480.06</v>
+      </c>
+      <c r="M59" s="631"/>
       <c r="N59" s="42"/>
       <c r="O59" s="392"/>
       <c r="P59" s="7"/>
@@ -33200,13 +33403,17 @@
       <c r="G60" s="137"/>
       <c r="H60" s="145"/>
       <c r="I60" s="80"/>
-      <c r="J60" s="325"/>
-      <c r="K60" s="467"/>
-      <c r="L60" s="458"/>
-      <c r="M60" s="591" t="s">
+      <c r="J60" s="325" t="s">
+        <v>826</v>
+      </c>
+      <c r="K60" s="658"/>
+      <c r="L60" s="458">
+        <v>2479.5</v>
+      </c>
+      <c r="M60" s="607" t="s">
         <v>719</v>
       </c>
-      <c r="N60" s="592"/>
+      <c r="N60" s="608"/>
       <c r="O60" s="392"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
@@ -33233,9 +33440,15 @@
       <c r="G61" s="137"/>
       <c r="H61" s="145"/>
       <c r="I61" s="80"/>
-      <c r="J61" s="325"/>
-      <c r="K61" s="468"/>
-      <c r="L61" s="6"/>
+      <c r="J61" s="325" t="s">
+        <v>826</v>
+      </c>
+      <c r="K61" s="468" t="s">
+        <v>583</v>
+      </c>
+      <c r="L61" s="6">
+        <v>7623.83</v>
+      </c>
       <c r="M61" s="41"/>
       <c r="N61" s="42"/>
       <c r="O61" s="392"/>
@@ -33333,13 +33546,13 @@
       <c r="I64" s="80"/>
       <c r="J64" s="325"/>
       <c r="K64" s="359"/>
-      <c r="L64" s="644" t="s">
+      <c r="L64" s="522" t="s">
         <v>822</v>
       </c>
-      <c r="M64" s="642">
+      <c r="M64" s="622">
         <v>-382722.22</v>
       </c>
-      <c r="N64" s="643"/>
+      <c r="N64" s="623"/>
       <c r="O64" s="392"/>
       <c r="P64" s="7"/>
       <c r="Q64" s="7"/>
@@ -33367,13 +33580,13 @@
       <c r="I65" s="80"/>
       <c r="J65" s="325"/>
       <c r="K65" s="467"/>
-      <c r="L65" s="644" t="s">
+      <c r="L65" s="522" t="s">
         <v>823</v>
       </c>
-      <c r="M65" s="646">
+      <c r="M65" s="624">
         <v>-163726</v>
       </c>
-      <c r="N65" s="647"/>
+      <c r="N65" s="625"/>
       <c r="O65" s="392"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
@@ -33404,12 +33617,12 @@
       <c r="J66" s="325"/>
       <c r="K66" s="468"/>
       <c r="L66" s="6"/>
-      <c r="M66" s="650">
+      <c r="M66" s="626">
         <f ca="1">SUM(M65+M64+M62)</f>
         <v>-583779.22</v>
       </c>
-      <c r="N66" s="651"/>
-      <c r="O66" s="652" t="s">
+      <c r="N66" s="627"/>
+      <c r="O66" s="632" t="s">
         <v>825</v>
       </c>
       <c r="P66" s="7"/>
@@ -33459,22 +33672,22 @@
       <c r="K67" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="L67" s="645">
+      <c r="L67" s="523">
         <f>SUM(L5:L66)</f>
-        <v>153963.14000000001</v>
-      </c>
-      <c r="M67" s="653"/>
-      <c r="N67" s="654"/>
-      <c r="O67" s="655"/>
+        <v>482695.31000000006</v>
+      </c>
+      <c r="M67" s="628"/>
+      <c r="N67" s="629"/>
+      <c r="O67" s="633"/>
       <c r="P67" s="366"/>
       <c r="Q67" s="366"/>
       <c r="R67" s="7">
         <f>SUM(R5:R66)</f>
-        <v>7281782.7999999998</v>
+        <v>7316251.5199999996</v>
       </c>
       <c r="S67" s="7">
         <f>SUM(S5:S66)</f>
-        <v>56844.140000000014</v>
+        <v>62688.140000000014</v>
       </c>
       <c r="T67" s="97"/>
       <c r="W67" s="210"/>
@@ -33497,16 +33710,16 @@
       <c r="A69" s="60"/>
       <c r="B69" s="100"/>
       <c r="C69" s="4"/>
-      <c r="H69" s="522" t="s">
+      <c r="H69" s="532" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="523"/>
+      <c r="I69" s="533"/>
       <c r="J69" s="101"/>
-      <c r="K69" s="524">
+      <c r="K69" s="534">
         <f>I67+L67</f>
-        <v>190109.14</v>
-      </c>
-      <c r="L69" s="525"/>
+        <v>518841.31000000006</v>
+      </c>
+      <c r="L69" s="535"/>
       <c r="M69" s="471"/>
       <c r="N69" s="472"/>
       <c r="O69" s="490"/>
@@ -33523,40 +33736,40 @@
       <c r="AG69" s="327"/>
     </row>
     <row r="70" spans="1:33" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="534" t="s">
+      <c r="D70" s="544" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="534"/>
+      <c r="E70" s="544"/>
       <c r="F70" s="103">
         <f>F67-K69-C67</f>
-        <v>2867958.5199999996</v>
+        <v>2539226.3499999996</v>
       </c>
       <c r="I70" s="104"/>
       <c r="J70" s="105"/>
-      <c r="R70" s="513">
+      <c r="R70" s="545">
         <f>R67+S67</f>
-        <v>7338626.9399999995</v>
-      </c>
-      <c r="S70" s="514"/>
+        <v>7378939.6599999992</v>
+      </c>
+      <c r="S70" s="546"/>
       <c r="U70" s="50"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="515" t="s">
+      <c r="D71" s="547" t="s">
         <v>502</v>
       </c>
-      <c r="E71" s="515"/>
+      <c r="E71" s="547"/>
       <c r="F71" s="95">
         <v>-2380713.08</v>
       </c>
-      <c r="I71" s="516" t="s">
+      <c r="I71" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J71" s="517"/>
-      <c r="K71" s="518">
+      <c r="J71" s="549"/>
+      <c r="K71" s="550">
         <f>F73+F74+F75</f>
-        <v>499431.43999999948</v>
-      </c>
-      <c r="L71" s="519"/>
+        <v>536310.85999999964</v>
+      </c>
+      <c r="L71" s="551"/>
       <c r="R71" s="50"/>
       <c r="U71" s="107"/>
     </row>
@@ -33583,18 +33796,18 @@
       </c>
       <c r="F73" s="95">
         <f>SUM(F70:F72)</f>
-        <v>487245.43999999948</v>
+        <v>158513.26999999955</v>
       </c>
       <c r="H73" s="34"/>
       <c r="I73" s="114" t="s">
         <v>21</v>
       </c>
       <c r="J73" s="115"/>
-      <c r="K73" s="520">
+      <c r="K73" s="552">
         <f>-C4</f>
         <v>-250140.85</v>
       </c>
-      <c r="L73" s="602"/>
+      <c r="L73" s="596"/>
       <c r="R73" s="50"/>
       <c r="S73" s="7"/>
       <c r="U73" s="50"/>
@@ -33617,22 +33830,22 @@
       <c r="C75" s="119">
         <v>44439</v>
       </c>
-      <c r="D75" s="528" t="s">
+      <c r="D75" s="538" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="529"/>
+      <c r="E75" s="539"/>
       <c r="F75" s="120">
-        <v>0</v>
-      </c>
-      <c r="I75" s="530" t="s">
+        <v>365611.59</v>
+      </c>
+      <c r="I75" s="540" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="531"/>
-      <c r="K75" s="532">
+      <c r="J75" s="541"/>
+      <c r="K75" s="542">
         <f>K71+K73</f>
-        <v>249290.58999999947</v>
-      </c>
-      <c r="L75" s="532"/>
+        <v>286170.00999999966</v>
+      </c>
+      <c r="L75" s="542"/>
       <c r="R75" s="50"/>
       <c r="S75" s="7"/>
       <c r="U75" s="121"/>
@@ -33647,10 +33860,10 @@
       <c r="S76" s="7"/>
     </row>
     <row r="77" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I77" s="611" t="s">
+      <c r="I77" s="634" t="s">
         <v>610</v>
       </c>
-      <c r="J77" s="612"/>
+      <c r="J77" s="635"/>
       <c r="K77" s="638">
         <v>37331</v>
       </c>
@@ -33663,8 +33876,8 @@
       <c r="C78" s="128"/>
       <c r="D78" s="129"/>
       <c r="E78" s="7"/>
-      <c r="I78" s="613"/>
-      <c r="J78" s="614"/>
+      <c r="I78" s="636"/>
+      <c r="J78" s="637"/>
       <c r="K78" s="640"/>
       <c r="L78" s="641"/>
       <c r="M78" s="2"/>
@@ -33718,7 +33931,7 @@
       <c r="C81" s="130"/>
       <c r="E81" s="7"/>
       <c r="M81" s="4"/>
-      <c r="AC81" s="582"/>
+      <c r="AC81" s="569"/>
       <c r="AD81" s="487"/>
       <c r="AE81" s="487"/>
       <c r="AF81" s="487"/>
@@ -33731,7 +33944,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="273"/>
       <c r="M82" s="4"/>
-      <c r="AC82" s="582"/>
+      <c r="AC82" s="569"/>
       <c r="AD82" s="487"/>
       <c r="AE82" s="487"/>
       <c r="AF82" s="487"/>
@@ -33828,37 +34041,6 @@
     <sortCondition ref="N45:N55"/>
   </sortState>
   <mergeCells count="41">
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="M65:N65"/>
-    <mergeCell ref="M66:N67"/>
-    <mergeCell ref="M58:M59"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="AC81:AC82"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="I77:J78"/>
-    <mergeCell ref="K77:L78"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="R70:S70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="M62:N63"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AE23:AF23"/>
-    <mergeCell ref="AE25:AF26"/>
-    <mergeCell ref="AG25:AG26"/>
-    <mergeCell ref="AB29:AB30"/>
-    <mergeCell ref="AC29:AC30"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="M60:N60"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:K1"/>
     <mergeCell ref="AB2:AG3"/>
@@ -33869,6 +34051,37 @@
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
+    <mergeCell ref="AB29:AB30"/>
+    <mergeCell ref="AC29:AC30"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AE23:AF23"/>
+    <mergeCell ref="AE25:AF26"/>
+    <mergeCell ref="AG25:AG26"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="R70:S70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="AC81:AC82"/>
+    <mergeCell ref="K73:L73"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="I77:J78"/>
+    <mergeCell ref="K77:L78"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M65:N65"/>
+    <mergeCell ref="M66:N67"/>
+    <mergeCell ref="M58:M59"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="M62:N63"/>
+    <mergeCell ref="M60:N60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -33884,8 +34097,8 @@
   </sheetPr>
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35428,12 +35641,12 @@
     <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="32"/>
-      <c r="B39" s="615" t="s">
+      <c r="B39" s="642" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="616"/>
-      <c r="D39" s="616"/>
-      <c r="E39" s="617"/>
+      <c r="C39" s="643"/>
+      <c r="D39" s="643"/>
+      <c r="E39" s="644"/>
       <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -36759,32 +36972,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="620" t="s">
+      <c r="B1" s="651" t="s">
         <v>726</v>
       </c>
-      <c r="C1" s="620"/>
-      <c r="D1" s="620"/>
-      <c r="E1" s="620"/>
-      <c r="H1" s="621" t="s">
+      <c r="C1" s="651"/>
+      <c r="D1" s="651"/>
+      <c r="E1" s="651"/>
+      <c r="H1" s="652" t="s">
         <v>726</v>
       </c>
-      <c r="I1" s="621"/>
-      <c r="J1" s="621"/>
+      <c r="I1" s="652"/>
+      <c r="J1" s="652"/>
       <c r="K1" s="205"/>
       <c r="L1" s="205"/>
       <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="620" t="s">
+      <c r="O1" s="651" t="s">
         <v>725</v>
       </c>
-      <c r="P1" s="620"/>
+      <c r="P1" s="651"/>
     </row>
     <row r="2" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="18"/>
       <c r="C2" s="4"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="556" t="s">
+      <c r="E2" s="570" t="s">
         <v>562</v>
       </c>
       <c r="F2" s="497"/>
@@ -36810,7 +37023,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="365"/>
-      <c r="E3" s="556"/>
+      <c r="E3" s="570"/>
       <c r="F3" s="497"/>
       <c r="H3" s="444">
         <v>126476.5</v>
@@ -36822,10 +37035,10 @@
         <v>44378</v>
       </c>
       <c r="K3" s="496"/>
-      <c r="L3" s="601" t="s">
+      <c r="L3" s="617" t="s">
         <v>567</v>
       </c>
-      <c r="M3" s="601"/>
+      <c r="M3" s="617"/>
       <c r="O3" s="444">
         <v>64006</v>
       </c>
@@ -37369,7 +37582,7 @@
         <v>44391</v>
       </c>
       <c r="K16" s="496"/>
-      <c r="L16" s="589">
+      <c r="L16" s="605">
         <f>SUM(L4:L15)</f>
         <v>3606750</v>
       </c>
@@ -37410,7 +37623,7 @@
         <v>44392</v>
       </c>
       <c r="K17" s="496"/>
-      <c r="L17" s="590"/>
+      <c r="L17" s="606"/>
       <c r="M17" s="476"/>
       <c r="O17" s="444">
         <v>0</v>
@@ -37483,10 +37696,10 @@
         <v>44394</v>
       </c>
       <c r="K19" s="496"/>
-      <c r="L19" s="591" t="s">
+      <c r="L19" s="607" t="s">
         <v>719</v>
       </c>
-      <c r="M19" s="592"/>
+      <c r="M19" s="608"/>
       <c r="O19" s="444">
         <v>0</v>
       </c>
@@ -37556,11 +37769,11 @@
         <v>44396</v>
       </c>
       <c r="K21" s="496"/>
-      <c r="L21" s="625">
+      <c r="L21" s="645">
         <f>L16-H37</f>
         <v>-383122.2200000002</v>
       </c>
-      <c r="M21" s="626"/>
+      <c r="M21" s="646"/>
       <c r="O21" s="444">
         <v>0</v>
       </c>
@@ -37594,8 +37807,8 @@
         <v>44397</v>
       </c>
       <c r="K22" s="496"/>
-      <c r="L22" s="627"/>
-      <c r="M22" s="628"/>
+      <c r="L22" s="647"/>
+      <c r="M22" s="648"/>
       <c r="O22" s="444">
         <v>0</v>
       </c>
@@ -37993,35 +38206,35 @@
       <c r="Q36" s="392"/>
     </row>
     <row r="37" spans="7:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="H37" s="597">
+      <c r="H37" s="613">
         <f>SUM(H3:H36)</f>
         <v>3989872.22</v>
       </c>
-      <c r="I37" s="599">
+      <c r="I37" s="615">
         <f>SUM(I3:I36)</f>
         <v>688820.5</v>
       </c>
       <c r="J37" s="496"/>
       <c r="K37" s="496"/>
       <c r="L37" s="496"/>
-      <c r="O37" s="597">
+      <c r="O37" s="613">
         <f>SUM(O3:O36)</f>
         <v>1464800.09</v>
       </c>
-      <c r="P37" s="599">
+      <c r="P37" s="615">
         <f>SUM(P3:P36)</f>
         <v>121896</v>
       </c>
       <c r="Q37" s="392"/>
     </row>
     <row r="38" spans="7:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H38" s="598"/>
-      <c r="I38" s="600"/>
+      <c r="H38" s="614"/>
+      <c r="I38" s="616"/>
       <c r="J38" s="496"/>
       <c r="K38" s="496"/>
       <c r="L38" s="496"/>
-      <c r="O38" s="598"/>
-      <c r="P38" s="600"/>
+      <c r="O38" s="614"/>
+      <c r="P38" s="616"/>
       <c r="Q38" s="392"/>
     </row>
     <row r="39" spans="7:17" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -38033,12 +38246,12 @@
     </row>
     <row r="40" spans="7:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G40" s="272"/>
-      <c r="H40" s="623"/>
-      <c r="I40" s="623"/>
-      <c r="O40" s="601" t="s">
+      <c r="H40" s="654"/>
+      <c r="I40" s="654"/>
+      <c r="O40" s="617" t="s">
         <v>567</v>
       </c>
-      <c r="P40" s="601"/>
+      <c r="P40" s="617"/>
       <c r="Q40" s="392"/>
     </row>
     <row r="41" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -38185,9 +38398,9 @@
     </row>
     <row r="53" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G53" s="272"/>
-      <c r="H53" s="624"/>
+      <c r="H53" s="655"/>
       <c r="I53" s="7"/>
-      <c r="O53" s="589">
+      <c r="O53" s="605">
         <f>SUM(O41:O52)</f>
         <v>1682687</v>
       </c>
@@ -38196,9 +38409,9 @@
     </row>
     <row r="54" spans="7:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G54" s="272"/>
-      <c r="H54" s="624"/>
+      <c r="H54" s="655"/>
       <c r="I54" s="7"/>
-      <c r="O54" s="590"/>
+      <c r="O54" s="606"/>
       <c r="P54" s="476"/>
       <c r="Q54" s="392"/>
     </row>
@@ -38212,12 +38425,12 @@
     </row>
     <row r="56" spans="7:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="G56" s="272"/>
-      <c r="H56" s="623"/>
-      <c r="I56" s="623"/>
-      <c r="O56" s="591" t="s">
+      <c r="H56" s="654"/>
+      <c r="I56" s="654"/>
+      <c r="O56" s="607" t="s">
         <v>719</v>
       </c>
-      <c r="P56" s="592"/>
+      <c r="P56" s="608"/>
       <c r="Q56" s="392"/>
     </row>
     <row r="57" spans="7:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -38230,8 +38443,8 @@
     </row>
     <row r="58" spans="7:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G58" s="272"/>
-      <c r="H58" s="622"/>
-      <c r="I58" s="622"/>
+      <c r="H58" s="653"/>
+      <c r="I58" s="653"/>
       <c r="O58" s="493">
         <f>O53-O37</f>
         <v>217886.90999999992</v>
@@ -38243,8 +38456,8 @@
     </row>
     <row r="59" spans="7:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G59" s="272"/>
-      <c r="H59" s="622"/>
-      <c r="I59" s="622"/>
+      <c r="H59" s="653"/>
+      <c r="I59" s="653"/>
       <c r="O59" s="506">
         <v>-383122.22</v>
       </c>
@@ -38272,24 +38485,14 @@
       <c r="P61" s="507"/>
     </row>
     <row r="62" spans="7:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="O62" s="618">
+      <c r="O62" s="649">
         <f>SUM(O58:O61)</f>
         <v>-328961.31000000006</v>
       </c>
-      <c r="P62" s="619"/>
+      <c r="P62" s="650"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O53:O54"/>
-    <mergeCell ref="O56:P56"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L21:M22"/>
-    <mergeCell ref="O62:P62"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L16:L17"/>
     <mergeCell ref="H58:I59"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="O37:O38"/>
@@ -38300,6 +38503,16 @@
     <mergeCell ref="H40:I40"/>
     <mergeCell ref="H53:H54"/>
     <mergeCell ref="H56:I56"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="O53:O54"/>
+    <mergeCell ref="O56:P56"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L21:M22"/>
+    <mergeCell ref="O62:P62"/>
   </mergeCells>
   <pageMargins left="0.37" right="0.13" top="0.43" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -38321,12 +38534,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32"/>
-      <c r="B1" s="615" t="s">
+      <c r="B1" s="642" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="616"/>
-      <c r="D1" s="616"/>
-      <c r="E1" s="617"/>
+      <c r="C1" s="643"/>
+      <c r="D1" s="643"/>
+      <c r="E1" s="644"/>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -38408,12 +38621,12 @@
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32"/>
-      <c r="B9" s="615" t="s">
+      <c r="B9" s="642" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="616"/>
-      <c r="D9" s="616"/>
-      <c r="E9" s="617"/>
+      <c r="C9" s="643"/>
+      <c r="D9" s="643"/>
+      <c r="E9" s="644"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -38569,12 +38782,12 @@
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32"/>
-      <c r="B20" s="615" t="s">
+      <c r="B20" s="642" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="616"/>
-      <c r="D20" s="616"/>
-      <c r="E20" s="617"/>
+      <c r="C20" s="643"/>
+      <c r="D20" s="643"/>
+      <c r="E20" s="644"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -38732,12 +38945,12 @@
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="32"/>
-      <c r="B31" s="615" t="s">
+      <c r="B31" s="642" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="616"/>
-      <c r="D31" s="616"/>
-      <c r="E31" s="617"/>
+      <c r="C31" s="643"/>
+      <c r="D31" s="643"/>
+      <c r="E31" s="644"/>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -38891,12 +39104,12 @@
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="32"/>
-      <c r="B42" s="615" t="s">
+      <c r="B42" s="642" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="616"/>
-      <c r="D42" s="616"/>
-      <c r="E42" s="617"/>
+      <c r="C42" s="643"/>
+      <c r="D42" s="643"/>
+      <c r="E42" s="644"/>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -39050,12 +39263,12 @@
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="32"/>
-      <c r="B54" s="615" t="s">
+      <c r="B54" s="642" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="616"/>
-      <c r="D54" s="616"/>
-      <c r="E54" s="617"/>
+      <c r="C54" s="643"/>
+      <c r="D54" s="643"/>
+      <c r="E54" s="644"/>
       <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -39296,17 +39509,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="535" t="s">
+      <c r="C1" s="524" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="535"/>
-      <c r="E1" s="535"/>
-      <c r="F1" s="535"/>
-      <c r="G1" s="535"/>
-      <c r="H1" s="535"/>
-      <c r="I1" s="535"/>
-      <c r="J1" s="535"/>
-      <c r="K1" s="535"/>
+      <c r="D1" s="524"/>
+      <c r="E1" s="524"/>
+      <c r="F1" s="524"/>
+      <c r="G1" s="524"/>
+      <c r="H1" s="524"/>
+      <c r="I1" s="524"/>
+      <c r="J1" s="524"/>
+      <c r="K1" s="524"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -39337,17 +39550,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="536" t="s">
+      <c r="B3" s="525" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="537"/>
+      <c r="C3" s="526"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="538" t="s">
+      <c r="H3" s="527" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="538"/>
+      <c r="I3" s="527"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -39376,14 +39589,14 @@
       <c r="D4" s="23">
         <v>44230</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="528" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="529"/>
+      <c r="H4" s="530" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="531"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -41922,61 +42135,61 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="522" t="s">
+      <c r="H64" s="532" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="523"/>
+      <c r="I64" s="533"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="524">
+      <c r="K64" s="534">
         <f>I62+L62</f>
         <v>259947.00000000003</v>
       </c>
-      <c r="L64" s="525"/>
-      <c r="M64" s="526">
+      <c r="L64" s="535"/>
+      <c r="M64" s="536">
         <f>M62+N62</f>
         <v>2744320</v>
       </c>
-      <c r="N64" s="527"/>
+      <c r="N64" s="537"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="534" t="s">
+      <c r="D65" s="544" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="534"/>
+      <c r="E65" s="544"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>2374814.2599999998</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="513">
+      <c r="P65" s="545">
         <f>P62+Q62</f>
         <v>3144691.75</v>
       </c>
-      <c r="Q65" s="514"/>
+      <c r="Q65" s="546"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="515" t="s">
+      <c r="D66" s="547" t="s">
         <v>18</v>
       </c>
-      <c r="E66" s="515"/>
+      <c r="E66" s="547"/>
       <c r="F66" s="95">
         <v>-2261593.1</v>
       </c>
-      <c r="I66" s="516" t="s">
+      <c r="I66" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="517"/>
-      <c r="K66" s="518">
+      <c r="J66" s="549"/>
+      <c r="K66" s="550">
         <f>F68+F69+F70</f>
         <v>355407.6199999997</v>
       </c>
-      <c r="L66" s="519"/>
+      <c r="L66" s="551"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
@@ -42013,11 +42226,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="520">
+      <c r="K68" s="552">
         <f>-C4</f>
         <v>-209541.1</v>
       </c>
-      <c r="L68" s="521"/>
+      <c r="L68" s="553"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -42041,22 +42254,22 @@
       <c r="C70" s="119">
         <v>44257</v>
       </c>
-      <c r="D70" s="528" t="s">
+      <c r="D70" s="538" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="529"/>
+      <c r="E70" s="539"/>
       <c r="F70" s="120">
         <v>223014.26</v>
       </c>
-      <c r="I70" s="530" t="s">
+      <c r="I70" s="540" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="531"/>
-      <c r="K70" s="532">
+      <c r="J70" s="541"/>
+      <c r="K70" s="542">
         <f>K66+K68</f>
         <v>145866.5199999997</v>
       </c>
-      <c r="L70" s="533"/>
+      <c r="L70" s="543"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -42157,6 +42370,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P65:Q65"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="I66:J66"/>
@@ -42168,12 +42387,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H64:I64"/>
     <mergeCell ref="K64:L64"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="D65:E65"/>
   </mergeCells>
   <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.51181102362204722" right="0.15748031496062992" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -43444,17 +43657,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="535" t="s">
+      <c r="C1" s="524" t="s">
         <v>429</v>
       </c>
-      <c r="D1" s="535"/>
-      <c r="E1" s="535"/>
-      <c r="F1" s="535"/>
-      <c r="G1" s="535"/>
-      <c r="H1" s="535"/>
-      <c r="I1" s="535"/>
-      <c r="J1" s="535"/>
-      <c r="K1" s="535"/>
+      <c r="D1" s="524"/>
+      <c r="E1" s="524"/>
+      <c r="F1" s="524"/>
+      <c r="G1" s="524"/>
+      <c r="H1" s="524"/>
+      <c r="I1" s="524"/>
+      <c r="J1" s="524"/>
+      <c r="K1" s="524"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -43484,17 +43697,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="536" t="s">
+      <c r="B3" s="525" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="537"/>
+      <c r="C3" s="526"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="538" t="s">
+      <c r="H3" s="527" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="538"/>
+      <c r="I3" s="527"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -43523,14 +43736,14 @@
       <c r="D4" s="23">
         <v>44257</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="528" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="529"/>
+      <c r="H4" s="530" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="531"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -46132,61 +46345,61 @@
       <c r="A62" s="60"/>
       <c r="B62" s="100"/>
       <c r="C62" s="4"/>
-      <c r="H62" s="522" t="s">
+      <c r="H62" s="532" t="s">
         <v>16</v>
       </c>
-      <c r="I62" s="523"/>
+      <c r="I62" s="533"/>
       <c r="J62" s="101"/>
-      <c r="K62" s="524">
+      <c r="K62" s="534">
         <f>I60+L60</f>
         <v>781851.32000000007</v>
       </c>
-      <c r="L62" s="525"/>
-      <c r="M62" s="526">
+      <c r="L62" s="535"/>
+      <c r="M62" s="536">
         <f>M60+N60</f>
         <v>4064802.5</v>
       </c>
-      <c r="N62" s="527"/>
+      <c r="N62" s="537"/>
       <c r="O62" s="102"/>
       <c r="P62" s="99"/>
       <c r="Q62" s="99"/>
       <c r="S62" s="174"/>
     </row>
     <row r="63" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="534" t="s">
+      <c r="D63" s="544" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="534"/>
+      <c r="E63" s="544"/>
       <c r="F63" s="103">
         <f>F60-K62-C60</f>
         <v>3177878.1399999997</v>
       </c>
       <c r="I63" s="104"/>
       <c r="J63" s="105"/>
-      <c r="P63" s="513">
+      <c r="P63" s="545">
         <f>P60+Q60</f>
         <v>4585432.34</v>
       </c>
-      <c r="Q63" s="514"/>
+      <c r="Q63" s="546"/>
       <c r="S63" s="50"/>
     </row>
     <row r="64" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="515" t="s">
+      <c r="D64" s="547" t="s">
         <v>18</v>
       </c>
-      <c r="E64" s="515"/>
+      <c r="E64" s="547"/>
       <c r="F64" s="95">
         <v>-3579271.89</v>
       </c>
-      <c r="I64" s="516" t="s">
+      <c r="I64" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J64" s="517"/>
-      <c r="K64" s="518">
+      <c r="J64" s="549"/>
+      <c r="K64" s="550">
         <f>F66+F67+F68</f>
         <v>-110332.85000000047</v>
       </c>
-      <c r="L64" s="519"/>
+      <c r="L64" s="551"/>
       <c r="P64" s="50"/>
       <c r="S64" s="107"/>
     </row>
@@ -46220,11 +46433,11 @@
         <v>21</v>
       </c>
       <c r="J66" s="115"/>
-      <c r="K66" s="520">
+      <c r="K66" s="552">
         <f>-C4</f>
         <v>-223014.26</v>
       </c>
-      <c r="L66" s="521"/>
+      <c r="L66" s="553"/>
       <c r="M66" s="116"/>
       <c r="P66" s="50"/>
       <c r="Q66" s="7"/>
@@ -46248,22 +46461,22 @@
       <c r="C68" s="119">
         <v>44291</v>
       </c>
-      <c r="D68" s="528" t="s">
+      <c r="D68" s="538" t="s">
         <v>24</v>
       </c>
-      <c r="E68" s="529"/>
+      <c r="E68" s="539"/>
       <c r="F68" s="120">
         <v>215362.9</v>
       </c>
-      <c r="I68" s="543" t="s">
+      <c r="I68" s="554" t="s">
         <v>431</v>
       </c>
-      <c r="J68" s="544"/>
-      <c r="K68" s="545">
+      <c r="J68" s="555"/>
+      <c r="K68" s="556">
         <f>K64+K66</f>
         <v>-333347.11000000045</v>
       </c>
-      <c r="L68" s="546"/>
+      <c r="L68" s="557"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
       <c r="S68" s="121"/>
@@ -46419,6 +46632,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="D63:E63"/>
     <mergeCell ref="P63:Q63"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="I64:J64"/>
@@ -46430,12 +46649,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H62:I62"/>
     <mergeCell ref="K62:L62"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="D63:E63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -47867,17 +48080,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="535" t="s">
+      <c r="C1" s="524" t="s">
         <v>430</v>
       </c>
-      <c r="D1" s="535"/>
-      <c r="E1" s="535"/>
-      <c r="F1" s="535"/>
-      <c r="G1" s="535"/>
-      <c r="H1" s="535"/>
-      <c r="I1" s="535"/>
-      <c r="J1" s="535"/>
-      <c r="K1" s="535"/>
+      <c r="D1" s="524"/>
+      <c r="E1" s="524"/>
+      <c r="F1" s="524"/>
+      <c r="G1" s="524"/>
+      <c r="H1" s="524"/>
+      <c r="I1" s="524"/>
+      <c r="J1" s="524"/>
+      <c r="K1" s="524"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -47907,17 +48120,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="536" t="s">
+      <c r="B3" s="525" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="537"/>
+      <c r="C3" s="526"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="538" t="s">
+      <c r="H3" s="527" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="538"/>
+      <c r="I3" s="527"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -47946,14 +48159,14 @@
       <c r="D4" s="23">
         <v>44291</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="528" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="529"/>
+      <c r="H4" s="530" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="548"/>
+      <c r="I4" s="558"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -50445,61 +50658,61 @@
       <c r="A58" s="60"/>
       <c r="B58" s="100"/>
       <c r="C58" s="4"/>
-      <c r="H58" s="522" t="s">
+      <c r="H58" s="532" t="s">
         <v>16</v>
       </c>
-      <c r="I58" s="523"/>
+      <c r="I58" s="533"/>
       <c r="J58" s="101"/>
-      <c r="K58" s="524">
+      <c r="K58" s="534">
         <f>I56+L56</f>
         <v>370346.35000000003</v>
       </c>
-      <c r="L58" s="549"/>
-      <c r="M58" s="526">
+      <c r="L58" s="559"/>
+      <c r="M58" s="536">
         <f>M56+N56</f>
         <v>3537422</v>
       </c>
-      <c r="N58" s="527"/>
+      <c r="N58" s="537"/>
       <c r="O58" s="102"/>
       <c r="P58" s="99"/>
       <c r="Q58" s="99"/>
       <c r="S58" s="174"/>
     </row>
     <row r="59" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="534" t="s">
+      <c r="D59" s="544" t="s">
         <v>17</v>
       </c>
-      <c r="E59" s="547"/>
+      <c r="E59" s="560"/>
       <c r="F59" s="103">
         <f>F56-K58-C56</f>
         <v>3048717.54</v>
       </c>
       <c r="I59" s="104"/>
       <c r="J59" s="105"/>
-      <c r="P59" s="513">
+      <c r="P59" s="545">
         <f>P56+Q56</f>
         <v>8073324.3200000003</v>
       </c>
-      <c r="Q59" s="514"/>
+      <c r="Q59" s="546"/>
       <c r="S59" s="50"/>
     </row>
     <row r="60" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="515" t="s">
+      <c r="D60" s="547" t="s">
         <v>18</v>
       </c>
-      <c r="E60" s="515"/>
+      <c r="E60" s="547"/>
       <c r="F60" s="95">
         <v>-3102716.28</v>
       </c>
-      <c r="I60" s="516" t="s">
+      <c r="I60" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J60" s="517"/>
-      <c r="K60" s="518">
+      <c r="J60" s="549"/>
+      <c r="K60" s="550">
         <f>F62+F63+F64</f>
         <v>216465.62000000023</v>
       </c>
-      <c r="L60" s="519"/>
+      <c r="L60" s="551"/>
       <c r="P60" s="50"/>
       <c r="S60" s="107"/>
     </row>
@@ -50533,11 +50746,11 @@
         <v>21</v>
       </c>
       <c r="J62" s="115"/>
-      <c r="K62" s="520">
+      <c r="K62" s="552">
         <f>-C4</f>
         <v>-215362.9</v>
       </c>
-      <c r="L62" s="521"/>
+      <c r="L62" s="553"/>
       <c r="M62" s="116"/>
       <c r="P62" s="50"/>
       <c r="Q62" s="7"/>
@@ -50561,22 +50774,22 @@
       <c r="C64" s="119">
         <v>44320</v>
       </c>
-      <c r="D64" s="528" t="s">
+      <c r="D64" s="538" t="s">
         <v>24</v>
       </c>
-      <c r="E64" s="529"/>
+      <c r="E64" s="539"/>
       <c r="F64" s="120">
         <v>249311.35999999999</v>
       </c>
-      <c r="I64" s="530" t="s">
+      <c r="I64" s="540" t="s">
         <v>25</v>
       </c>
-      <c r="J64" s="531"/>
-      <c r="K64" s="532">
+      <c r="J64" s="541"/>
+      <c r="K64" s="542">
         <f>K60+K62</f>
         <v>1102.720000000234</v>
       </c>
-      <c r="L64" s="533"/>
+      <c r="L64" s="543"/>
       <c r="P64" s="50"/>
       <c r="Q64" s="7"/>
       <c r="S64" s="121"/>
@@ -50732,6 +50945,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="D59:E59"/>
     <mergeCell ref="P59:Q59"/>
     <mergeCell ref="D60:E60"/>
     <mergeCell ref="I60:J60"/>
@@ -50743,12 +50962,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H58:I58"/>
     <mergeCell ref="K58:L58"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="M58:N58"/>
-    <mergeCell ref="D59:E59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -51631,17 +51844,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="535" t="s">
+      <c r="C1" s="524" t="s">
         <v>504</v>
       </c>
-      <c r="D1" s="535"/>
-      <c r="E1" s="535"/>
-      <c r="F1" s="535"/>
-      <c r="G1" s="535"/>
-      <c r="H1" s="535"/>
-      <c r="I1" s="535"/>
-      <c r="J1" s="535"/>
-      <c r="K1" s="535"/>
+      <c r="D1" s="524"/>
+      <c r="E1" s="524"/>
+      <c r="F1" s="524"/>
+      <c r="G1" s="524"/>
+      <c r="H1" s="524"/>
+      <c r="I1" s="524"/>
+      <c r="J1" s="524"/>
+      <c r="K1" s="524"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
       <c r="U1" s="209"/>
@@ -51671,17 +51884,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="536" t="s">
+      <c r="B3" s="525" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="537"/>
+      <c r="C3" s="526"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="H3" s="538" t="s">
+      <c r="H3" s="527" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="538"/>
+      <c r="I3" s="527"/>
       <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
@@ -51710,14 +51923,14 @@
       <c r="D4" s="23">
         <v>44320</v>
       </c>
-      <c r="E4" s="539" t="s">
+      <c r="E4" s="528" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="540"/>
-      <c r="H4" s="541" t="s">
+      <c r="F4" s="529"/>
+      <c r="H4" s="530" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="542"/>
+      <c r="I4" s="531"/>
       <c r="J4" s="24"/>
       <c r="K4" s="25"/>
       <c r="L4" s="26"/>
@@ -54594,71 +54807,71 @@
       <c r="A64" s="60"/>
       <c r="B64" s="100"/>
       <c r="C64" s="4"/>
-      <c r="H64" s="522" t="s">
+      <c r="H64" s="532" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="523"/>
+      <c r="I64" s="533"/>
       <c r="J64" s="101"/>
-      <c r="K64" s="524">
+      <c r="K64" s="534">
         <f>I62+L62</f>
         <v>779034.56000000017</v>
       </c>
-      <c r="L64" s="525"/>
-      <c r="M64" s="526">
+      <c r="L64" s="535"/>
+      <c r="M64" s="536">
         <f>M62+N62</f>
         <v>4478181</v>
       </c>
-      <c r="N64" s="527"/>
+      <c r="N64" s="537"/>
       <c r="O64" s="102"/>
       <c r="P64" s="99"/>
       <c r="Q64" s="99"/>
       <c r="S64" s="174"/>
     </row>
     <row r="65" spans="2:19" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="534" t="s">
+      <c r="D65" s="544" t="s">
         <v>17</v>
       </c>
-      <c r="E65" s="534"/>
+      <c r="E65" s="544"/>
       <c r="F65" s="103">
         <f>F62-K64-C62</f>
         <v>3602842.44</v>
       </c>
       <c r="I65" s="104"/>
       <c r="J65" s="105"/>
-      <c r="P65" s="513">
+      <c r="P65" s="545">
         <f>P62+Q62</f>
         <v>5004562.5599999996</v>
       </c>
-      <c r="Q65" s="514"/>
+      <c r="Q65" s="546"/>
       <c r="S65" s="50"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="550" t="s">
+      <c r="B66" s="561" t="s">
         <v>528</v>
       </c>
-      <c r="C66" s="551"/>
-      <c r="D66" s="534" t="s">
+      <c r="C66" s="562"/>
+      <c r="D66" s="544" t="s">
         <v>502</v>
       </c>
-      <c r="E66" s="534"/>
+      <c r="E66" s="544"/>
       <c r="F66" s="95">
         <v>-3854423.8</v>
       </c>
-      <c r="I66" s="516" t="s">
+      <c r="I66" s="548" t="s">
         <v>19</v>
       </c>
-      <c r="J66" s="517"/>
-      <c r="K66" s="518">
+      <c r="J66" s="549"/>
+      <c r="K66" s="550">
         <f>F68+F69+F70</f>
         <v>14998.430000000139</v>
       </c>
-      <c r="L66" s="519"/>
+      <c r="L66" s="551"/>
       <c r="P66" s="50"/>
       <c r="S66" s="107"/>
     </row>
     <row r="67" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="552"/>
-      <c r="C67" s="553"/>
+      <c r="B67" s="563"/>
+      <c r="C67" s="564"/>
       <c r="D67" s="108"/>
       <c r="E67" s="60"/>
       <c r="F67" s="109">
@@ -54673,8 +54886,8 @@
       <c r="S67" s="50"/>
     </row>
     <row r="68" spans="2:19" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="554"/>
-      <c r="C68" s="555"/>
+      <c r="B68" s="565"/>
+      <c r="C68" s="566"/>
       <c r="E68" s="60" t="s">
         <v>20</v>
       </c>
@@ -54687,11 +54900,11 @@
         <v>21</v>
       </c>
       <c r="J68" s="115"/>
-      <c r="K68" s="520">
+      <c r="K68" s="552">
         <f>-C4</f>
         <v>-249311.35999999999</v>
       </c>
-      <c r="L68" s="521"/>
+      <c r="L68" s="553"/>
       <c r="M68" s="116"/>
       <c r="P68" s="50"/>
       <c r="Q68" s="7"/>
@@ -54715,22 +54928,22 @@
       <c r="C70" s="119">
         <v>44353</v>
       </c>
-      <c r="D70" s="528" t="s">
+      <c r="D70" s="538" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="529"/>
+      <c r="E70" s="539"/>
       <c r="F70" s="120">
         <v>255764.39</v>
       </c>
-      <c r="I70" s="530" t="s">
+      <c r="I70" s="540" t="s">
         <v>431</v>
       </c>
-      <c r="J70" s="531"/>
-      <c r="K70" s="532">
+      <c r="J70" s="541"/>
+      <c r="K70" s="542">
         <f>K66+K68</f>
         <v>-234312.92999999985</v>
       </c>
-      <c r="L70" s="533"/>
+      <c r="L70" s="543"/>
       <c r="P70" s="50"/>
       <c r="Q70" s="7"/>
       <c r="S70" s="121"/>
@@ -54886,6 +55099,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="D65:E65"/>
     <mergeCell ref="P65:Q65"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="I66:J66"/>
@@ -54899,11 +55117,6 @@
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="B66:C68"/>
     <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="D65:E65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>